<commit_message>
prepare seeds and modify models structure, feed users and populate them
</commit_message>
<xml_diff>
--- a/src/seeds/files/002_MalaUva_SeedFile.xlsx
+++ b/src/seeds/files/002_MalaUva_SeedFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nama/Library/CloudStorage/Dropbox/00-WF-C/2-NAMA/ROCKTHECODE/CODE/02-deliverables/22_RTC_P13_backend-react/malauva-backend/src/seeds/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D3363E-E0EC-B04E-A1DB-86F0413BCCAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8016AC81-5222-4346-9540-FDEC04CE7746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="25700" activeTab="1" xr2:uid="{52677FAD-7042-B148-9A25-30607DD347FB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="672">
   <si>
     <t>name</t>
   </si>
@@ -5001,6 +5001,9 @@
   </si>
   <si>
     <t>role</t>
+  </si>
+  <si>
+    <t>4000 4065</t>
   </si>
 </sst>
 </file>
@@ -5483,7 +5486,7 @@
       </c>
       <c r="J2" s="1">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -5516,7 +5519,7 @@
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J66" ca="1" si="0">RANDBETWEEN(0,100)</f>
-        <v>14</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -5549,7 +5552,7 @@
       </c>
       <c r="J4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -5582,7 +5585,7 @@
       </c>
       <c r="J5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -5615,7 +5618,7 @@
       </c>
       <c r="J6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -5648,7 +5651,7 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -5681,7 +5684,7 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -5714,7 +5717,7 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -5747,7 +5750,7 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -5780,7 +5783,7 @@
       </c>
       <c r="J11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -5813,7 +5816,7 @@
       </c>
       <c r="J12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -5846,7 +5849,7 @@
       </c>
       <c r="J13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -5879,7 +5882,7 @@
       </c>
       <c r="J14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -5912,7 +5915,7 @@
       </c>
       <c r="J15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -5945,7 +5948,7 @@
       </c>
       <c r="J16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -5978,7 +5981,7 @@
       </c>
       <c r="J17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -6011,7 +6014,7 @@
       </c>
       <c r="J18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -6044,7 +6047,7 @@
       </c>
       <c r="J19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -6077,7 +6080,7 @@
       </c>
       <c r="J20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -6110,7 +6113,7 @@
       </c>
       <c r="J21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -6143,7 +6146,7 @@
       </c>
       <c r="J22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -6176,7 +6179,7 @@
       </c>
       <c r="J23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -6209,7 +6212,7 @@
       </c>
       <c r="J24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -6242,7 +6245,7 @@
       </c>
       <c r="J25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -6275,7 +6278,7 @@
       </c>
       <c r="J26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -6308,7 +6311,7 @@
       </c>
       <c r="J27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -6341,7 +6344,7 @@
       </c>
       <c r="J28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -6374,7 +6377,7 @@
       </c>
       <c r="J29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -6407,7 +6410,7 @@
       </c>
       <c r="J30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -6440,7 +6443,7 @@
       </c>
       <c r="J31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -6473,7 +6476,7 @@
       </c>
       <c r="J32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -6506,7 +6509,7 @@
       </c>
       <c r="J33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -6539,7 +6542,7 @@
       </c>
       <c r="J34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -6572,7 +6575,7 @@
       </c>
       <c r="J35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -6605,7 +6608,7 @@
       </c>
       <c r="J36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -6638,7 +6641,7 @@
       </c>
       <c r="J37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -6671,7 +6674,7 @@
       </c>
       <c r="J38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -6704,7 +6707,7 @@
       </c>
       <c r="J39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -6770,7 +6773,7 @@
       </c>
       <c r="J41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -6803,7 +6806,7 @@
       </c>
       <c r="J42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -6836,7 +6839,7 @@
       </c>
       <c r="J43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -6869,7 +6872,7 @@
       </c>
       <c r="J44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -6902,7 +6905,7 @@
       </c>
       <c r="J45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -6935,7 +6938,7 @@
       </c>
       <c r="J46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -6968,7 +6971,7 @@
       </c>
       <c r="J47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -7001,7 +7004,7 @@
       </c>
       <c r="J48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -7034,7 +7037,7 @@
       </c>
       <c r="J49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -7067,7 +7070,7 @@
       </c>
       <c r="J50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -7100,7 +7103,7 @@
       </c>
       <c r="J51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -7133,7 +7136,7 @@
       </c>
       <c r="J52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -7166,7 +7169,7 @@
       </c>
       <c r="J53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -7199,7 +7202,7 @@
       </c>
       <c r="J54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -7232,7 +7235,7 @@
       </c>
       <c r="J55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -7265,7 +7268,7 @@
       </c>
       <c r="J56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -7298,7 +7301,7 @@
       </c>
       <c r="J57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -7331,7 +7334,7 @@
       </c>
       <c r="J58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -7364,7 +7367,7 @@
       </c>
       <c r="J59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -7397,7 +7400,7 @@
       </c>
       <c r="J60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -7430,7 +7433,7 @@
       </c>
       <c r="J61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -7463,7 +7466,7 @@
       </c>
       <c r="J62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -7496,7 +7499,7 @@
       </c>
       <c r="J63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -7529,7 +7532,7 @@
       </c>
       <c r="J64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -7562,7 +7565,7 @@
       </c>
       <c r="J65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -7595,7 +7598,7 @@
       </c>
       <c r="J66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -7628,7 +7631,7 @@
       </c>
       <c r="J67" s="1">
         <f t="shared" ref="J67:J120" ca="1" si="1">RANDBETWEEN(0,100)</f>
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -7661,7 +7664,7 @@
       </c>
       <c r="J68" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -7694,7 +7697,7 @@
       </c>
       <c r="J69" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
@@ -7727,7 +7730,7 @@
       </c>
       <c r="J70" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -7760,7 +7763,7 @@
       </c>
       <c r="J71" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -7793,7 +7796,7 @@
       </c>
       <c r="J72" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -7826,7 +7829,7 @@
       </c>
       <c r="J73" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -7859,7 +7862,7 @@
       </c>
       <c r="J74" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -7892,7 +7895,7 @@
       </c>
       <c r="J75" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
@@ -7925,7 +7928,7 @@
       </c>
       <c r="J76" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
@@ -7991,7 +7994,7 @@
       </c>
       <c r="J78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
@@ -8024,7 +8027,7 @@
       </c>
       <c r="J79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
@@ -8057,7 +8060,7 @@
       </c>
       <c r="J80" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -8090,7 +8093,7 @@
       </c>
       <c r="J81" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
@@ -8156,7 +8159,7 @@
       </c>
       <c r="J83" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
@@ -8189,7 +8192,7 @@
       </c>
       <c r="J84" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
@@ -8255,7 +8258,7 @@
       </c>
       <c r="J86" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>75</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
@@ -8288,7 +8291,7 @@
       </c>
       <c r="J87" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
@@ -8321,7 +8324,7 @@
       </c>
       <c r="J88" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
@@ -8354,7 +8357,7 @@
       </c>
       <c r="J89" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
@@ -8387,7 +8390,7 @@
       </c>
       <c r="J90" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
@@ -8420,7 +8423,7 @@
       </c>
       <c r="J91" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>57</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
@@ -8453,7 +8456,7 @@
       </c>
       <c r="J92" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
@@ -8486,7 +8489,7 @@
       </c>
       <c r="J93" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
@@ -8519,7 +8522,7 @@
       </c>
       <c r="J94" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
@@ -8552,7 +8555,7 @@
       </c>
       <c r="J95" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
@@ -8585,7 +8588,7 @@
       </c>
       <c r="J96" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
@@ -8618,7 +8621,7 @@
       </c>
       <c r="J97" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
@@ -8651,7 +8654,7 @@
       </c>
       <c r="J98" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
@@ -8684,7 +8687,7 @@
       </c>
       <c r="J99" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
@@ -8717,7 +8720,7 @@
       </c>
       <c r="J100" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
@@ -8750,7 +8753,7 @@
       </c>
       <c r="J101" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
@@ -8783,7 +8786,7 @@
       </c>
       <c r="J102" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
@@ -8816,7 +8819,7 @@
       </c>
       <c r="J103" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
@@ -8849,7 +8852,7 @@
       </c>
       <c r="J104" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
@@ -8882,7 +8885,7 @@
       </c>
       <c r="J105" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
@@ -8915,7 +8918,7 @@
       </c>
       <c r="J106" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
@@ -8948,7 +8951,7 @@
       </c>
       <c r="J107" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>48</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
@@ -8981,7 +8984,7 @@
       </c>
       <c r="J108" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>94</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
@@ -9014,7 +9017,7 @@
       </c>
       <c r="J109" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
@@ -9047,7 +9050,7 @@
       </c>
       <c r="J110" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
@@ -9080,7 +9083,7 @@
       </c>
       <c r="J111" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
@@ -9113,7 +9116,7 @@
       </c>
       <c r="J112" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>63</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
@@ -9146,7 +9149,7 @@
       </c>
       <c r="J113" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
@@ -9179,7 +9182,7 @@
       </c>
       <c r="J114" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
@@ -9212,7 +9215,7 @@
       </c>
       <c r="J115" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
@@ -9245,7 +9248,7 @@
       </c>
       <c r="J116" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
@@ -9278,7 +9281,7 @@
       </c>
       <c r="J117" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>43</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
@@ -9311,7 +9314,7 @@
       </c>
       <c r="J118" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
@@ -9344,7 +9347,7 @@
       </c>
       <c r="J119" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
@@ -9377,7 +9380,7 @@
       </c>
       <c r="J120" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
@@ -9421,10 +9424,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F341AF76-375D-CC4F-BE34-40B60AD74311}">
-  <dimension ref="A1:L123"/>
+  <dimension ref="A1:L194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H57" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="H54" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9498,20 +9501,19 @@
       <c r="E2" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="F2" s="1">
-        <f ca="1">RANDBETWEEN(0,100) + 4000</f>
-        <v>4084</v>
+      <c r="F2" s="1" t="s">
+        <v>671</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>237</v>
       </c>
       <c r="I2" s="1">
         <f t="shared" ref="I2:I66" ca="1" si="0">RANDBETWEEN(1,100) ^ 3 + 4050000</f>
-        <v>4439017</v>
+        <v>4051728</v>
       </c>
       <c r="L2" s="1">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>64</v>
+        <f ca="1">RANDBETWEEN(1,100) + 1000</f>
+        <v>1082</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9532,18 +9534,18 @@
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F66" ca="1" si="1">RANDBETWEEN(0,100) + 4000</f>
-        <v>4057</v>
+        <v>4029</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>238</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4991192</v>
+        <v>4067576</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L66" ca="1" si="2">RANDBETWEEN(1,100)</f>
-        <v>69</v>
+        <f t="shared" ref="L3:L66" ca="1" si="2">RANDBETWEEN(1,100) + 1000</f>
+        <v>1100</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9564,18 +9566,18 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4076</v>
+        <v>4006</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>239</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050216</v>
+        <v>4100653</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9596,18 +9598,18 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4082</v>
+        <v>4021</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>240</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4190608</v>
+        <v>4059261</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9628,18 +9630,18 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4094</v>
+        <v>4091</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>241</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4082768</v>
+        <v>4621787</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9660,18 +9662,18 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4085</v>
+        <v>4018</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>242</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4731472</v>
+        <v>4160592</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>81</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9692,18 +9694,18 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4017</v>
+        <v>4076</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>243</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4276981</v>
+        <v>4488976</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>82</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9724,18 +9726,18 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4068</v>
+        <v>4095</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>244</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4245112</v>
+        <v>4288328</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>89</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9756,18 +9758,18 @@
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4027</v>
+        <v>4098</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>245</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4089304</v>
+        <v>4907375</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>47</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9788,18 +9790,18 @@
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4005</v>
+        <v>4063</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>246</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4141125</v>
+        <v>4055832</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>98</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9819,19 +9821,19 @@
         <v>236</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>4083</v>
+        <f ca="1">RANDBETWEEN(0,100) + 4000</f>
+        <v>4011</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>247</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4312144</v>
+        <v>5050000</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>89</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9852,18 +9854,18 @@
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4030</v>
+        <v>4018</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>248</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4245112</v>
+        <v>4055832</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>72</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9884,18 +9886,18 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4062</v>
+        <v>4002</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>249</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050512</v>
+        <v>4051331</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9916,7 +9918,7 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4052</v>
+        <v>4019</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>250</v>
@@ -9927,7 +9929,7 @@
       </c>
       <c r="L15" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>50</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9948,18 +9950,18 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4017</v>
+        <v>4012</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>251</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4686056</v>
+        <v>4266000</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>66</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9980,7 +9982,7 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4064</v>
+        <v>4009</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>252</v>
@@ -9991,7 +9993,7 @@
       </c>
       <c r="L17" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10012,18 +10014,18 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4009</v>
+        <v>4066</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>253</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4488976</v>
+        <v>4378509</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>97</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10044,18 +10046,18 @@
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4087</v>
+        <v>4045</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>254</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4059261</v>
+        <v>4050001</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10076,18 +10078,18 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4087</v>
+        <v>4029</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>255</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4190608</v>
+        <v>4378509</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>92</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10108,18 +10110,18 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4048</v>
+        <v>4065</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>256</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4266000</v>
+        <v>4141125</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>70</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10140,18 +10142,18 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4016</v>
+        <v>4027</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>257</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4300047</v>
+        <v>4190608</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10172,18 +10174,18 @@
       </c>
       <c r="F23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4075</v>
+        <v>4072</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>258</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4051728</v>
+        <v>4562000</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>95</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10204,18 +10206,18 @@
       </c>
       <c r="F24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4076</v>
+        <v>4088</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>259</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4085937</v>
+        <v>4050027</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10236,18 +10238,18 @@
       </c>
       <c r="F25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4065</v>
+        <v>4084</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>260</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4052197</v>
+        <v>4337496</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10268,18 +10270,18 @@
       </c>
       <c r="F26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4015</v>
+        <v>4029</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>261</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4055832</v>
+        <v>4104872</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>58</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10300,18 +10302,18 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4076</v>
+        <v>4063</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>262</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4071952</v>
+        <v>4324625</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>50</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10332,18 +10334,18 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4014</v>
+        <v>4085</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>263</v>
       </c>
       <c r="I28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4621787</v>
+        <v>4153823</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>72</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10364,18 +10366,18 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4046</v>
+        <v>4018</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>264</v>
       </c>
       <c r="I29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050512</v>
+        <v>4052197</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>47</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10396,18 +10398,18 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4045</v>
+        <v>4001</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>265</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4092875</v>
+        <v>4880584</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>82</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10428,18 +10430,18 @@
       </c>
       <c r="F31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4082</v>
+        <v>4006</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>266</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4074389</v>
+        <v>4393000</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>48</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10460,18 +10462,18 @@
       </c>
       <c r="F32" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4069</v>
+        <v>4012</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>267</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4147336</v>
+        <v>4051000</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>68</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10492,18 +10494,18 @@
       </c>
       <c r="F33" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4078</v>
+        <v>4098</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>268</v>
       </c>
       <c r="I33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4065625</v>
+        <v>4051728</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>57</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10524,18 +10526,18 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4022</v>
+        <v>4099</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>269</v>
       </c>
       <c r="I34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4054913</v>
+        <v>4581441</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10556,18 +10558,18 @@
       </c>
       <c r="F35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4038</v>
+        <v>4027</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>270</v>
       </c>
       <c r="I35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4069683</v>
+        <v>4300047</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10595,11 +10597,11 @@
       </c>
       <c r="I36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4854357</v>
+        <v>4153823</v>
       </c>
       <c r="L36" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>73</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10620,18 +10622,18 @@
       </c>
       <c r="F37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4099</v>
+        <v>4090</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>272</v>
       </c>
       <c r="I37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4601368</v>
+        <v>4050064</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10652,18 +10654,18 @@
       </c>
       <c r="F38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4081</v>
+        <v>4010</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>273</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4207464</v>
+        <v>4664125</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>98</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10684,18 +10686,18 @@
       </c>
       <c r="F39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4003</v>
+        <v>4031</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>274</v>
       </c>
       <c r="I39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4056859</v>
+        <v>4216375</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10716,18 +10718,18 @@
       </c>
       <c r="F40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4031</v>
+        <v>4085</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>275</v>
       </c>
       <c r="I40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4255379</v>
+        <v>4225616</v>
       </c>
       <c r="L40" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>67</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10748,18 +10750,18 @@
       </c>
       <c r="F41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4021</v>
+        <v>4096</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>276</v>
       </c>
       <c r="I41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050216</v>
+        <v>4543039</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10780,18 +10782,18 @@
       </c>
       <c r="F42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4075</v>
+        <v>4076</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>277</v>
       </c>
       <c r="I42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4065625</v>
+        <v>4129507</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>66</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10812,18 +10814,18 @@
       </c>
       <c r="F43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4035</v>
+        <v>4068</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>278</v>
       </c>
       <c r="I43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4054096</v>
+        <v>4324625</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10844,18 +10846,18 @@
       </c>
       <c r="F44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4022</v>
+        <v>4012</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>279</v>
       </c>
       <c r="I44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4124088</v>
+        <v>4055832</v>
       </c>
       <c r="L44" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>51</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10876,18 +10878,18 @@
       </c>
       <c r="F45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4068</v>
+        <v>4062</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>280</v>
       </c>
       <c r="I45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4167649</v>
+        <v>4962673</v>
       </c>
       <c r="L45" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>90</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10908,18 +10910,18 @@
       </c>
       <c r="F46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4095</v>
+        <v>4058</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>281</v>
       </c>
       <c r="I46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4051331</v>
+        <v>4907375</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>84</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10940,18 +10942,18 @@
       </c>
       <c r="F47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4054</v>
+        <v>4008</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>282</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4065625</v>
+        <v>4160592</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>40</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10972,18 +10974,18 @@
       </c>
       <c r="F48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4087</v>
+        <v>4035</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>283</v>
       </c>
       <c r="I48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4731472</v>
+        <v>4082768</v>
       </c>
       <c r="L48" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11004,18 +11006,18 @@
       </c>
       <c r="F49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4042</v>
+        <v>4028</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>284</v>
       </c>
       <c r="I49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4225616</v>
+        <v>4288328</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11036,18 +11038,18 @@
       </c>
       <c r="F50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4039</v>
+        <v>4005</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>285</v>
       </c>
       <c r="I50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4135184</v>
+        <v>4190608</v>
       </c>
       <c r="L50" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11068,18 +11070,18 @@
       </c>
       <c r="F51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4093</v>
+        <v>4071</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>286</v>
       </c>
       <c r="I51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050512</v>
+        <v>4276981</v>
       </c>
       <c r="L51" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>82</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11100,18 +11102,18 @@
       </c>
       <c r="F52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4008</v>
+        <v>4082</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4803571</v>
+        <v>4562000</v>
       </c>
       <c r="L52" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>65</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11132,18 +11134,18 @@
       </c>
       <c r="F53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4089</v>
+        <v>4025</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>288</v>
       </c>
       <c r="I53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4378509</v>
+        <v>4216375</v>
       </c>
       <c r="L53" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>79</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11164,18 +11166,18 @@
       </c>
       <c r="F54" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4089</v>
+        <v>4090</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>289</v>
       </c>
       <c r="I54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4581441</v>
+        <v>4779000</v>
       </c>
       <c r="L54" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>81</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11196,18 +11198,18 @@
       </c>
       <c r="F55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4085</v>
+        <v>4081</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>290</v>
       </c>
       <c r="I55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4803571</v>
+        <v>4276981</v>
       </c>
       <c r="L55" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>40</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11228,18 +11230,18 @@
       </c>
       <c r="F56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4036</v>
+        <v>4086</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>291</v>
       </c>
       <c r="I56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4312144</v>
+        <v>4053375</v>
       </c>
       <c r="L56" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11260,18 +11262,18 @@
       </c>
       <c r="F57" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4012</v>
+        <v>4005</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>292</v>
       </c>
       <c r="I57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4051000</v>
+        <v>4393000</v>
       </c>
       <c r="L57" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>39</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11292,18 +11294,18 @@
       </c>
       <c r="F58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4001</v>
+        <v>4006</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>293</v>
       </c>
       <c r="I58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4708503</v>
+        <v>4378509</v>
       </c>
       <c r="L58" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>54</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11324,18 +11326,18 @@
       </c>
       <c r="F59" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4038</v>
+        <v>4016</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>294</v>
       </c>
       <c r="I59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4300047</v>
+        <v>4423248</v>
       </c>
       <c r="L59" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11356,18 +11358,18 @@
       </c>
       <c r="F60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4048</v>
+        <v>4001</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>295</v>
       </c>
       <c r="I60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4124088</v>
+        <v>4803571</v>
       </c>
       <c r="L60" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11388,18 +11390,18 @@
       </c>
       <c r="F61" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4069</v>
+        <v>4060</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>296</v>
       </c>
       <c r="I61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4337496</v>
+        <v>4089304</v>
       </c>
       <c r="L61" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11420,18 +11422,18 @@
       </c>
       <c r="F62" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4019</v>
+        <v>4098</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>297</v>
       </c>
       <c r="I62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4300047</v>
+        <v>4524552</v>
       </c>
       <c r="L62" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11452,18 +11454,18 @@
       </c>
       <c r="F63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4010</v>
+        <v>4053</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>298</v>
       </c>
       <c r="I63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4077000</v>
+        <v>4050216</v>
       </c>
       <c r="L63" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11484,18 +11486,18 @@
       </c>
       <c r="F64" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4100</v>
+        <v>4087</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>299</v>
       </c>
       <c r="I64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4854357</v>
+        <v>4050125</v>
       </c>
       <c r="L64" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>55</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11516,18 +11518,18 @@
       </c>
       <c r="F65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4087</v>
+        <v>4027</v>
       </c>
       <c r="H65" s="4" t="s">
         <v>300</v>
       </c>
       <c r="I65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4056859</v>
+        <v>4803571</v>
       </c>
       <c r="L65" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11548,18 +11550,18 @@
       </c>
       <c r="F66" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4037</v>
+        <v>4060</v>
       </c>
       <c r="H66" s="4" t="s">
         <v>301</v>
       </c>
       <c r="I66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4135184</v>
+        <v>4350763</v>
       </c>
       <c r="L66" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11580,18 +11582,18 @@
       </c>
       <c r="F67" s="1">
         <f t="shared" ref="F67:F111" ca="1" si="3">RANDBETWEEN(0,100) + 4000</f>
-        <v>4068</v>
+        <v>4044</v>
       </c>
       <c r="H67" s="4" t="s">
         <v>302</v>
       </c>
       <c r="I67" s="1">
         <f t="shared" ref="I67:I111" ca="1" si="4">RANDBETWEEN(1,100) ^ 3 + 4050000</f>
-        <v>4378509</v>
+        <v>4581441</v>
       </c>
       <c r="L67" s="1">
-        <f t="shared" ref="L67:L111" ca="1" si="5">RANDBETWEEN(1,100)</f>
-        <v>36</v>
+        <f t="shared" ref="L67:L111" ca="1" si="5">RANDBETWEEN(1,100) + 1000</f>
+        <v>1090</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11612,18 +11614,18 @@
       </c>
       <c r="F68" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4063</v>
+        <v>4041</v>
       </c>
       <c r="H68" s="4" t="s">
         <v>303</v>
       </c>
       <c r="I68" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>5020299</v>
+        <v>4124088</v>
       </c>
       <c r="L68" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>66</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11644,18 +11646,18 @@
       </c>
       <c r="F69" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4035</v>
+        <v>4000</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>304</v>
       </c>
       <c r="I69" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4050343</v>
+        <v>4054913</v>
       </c>
       <c r="L69" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>83</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11676,18 +11678,18 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4011</v>
+        <v>4075</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>305</v>
       </c>
       <c r="I70" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4160592</v>
+        <v>4439017</v>
       </c>
       <c r="L70" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>66</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11708,18 +11710,18 @@
       </c>
       <c r="F71" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4100</v>
+        <v>4092</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>306</v>
       </c>
       <c r="I71" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4118921</v>
+        <v>4089304</v>
       </c>
       <c r="L71" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>96</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11740,7 +11742,7 @@
       </c>
       <c r="F72" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4069</v>
+        <v>4013</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>307</v>
@@ -11751,7 +11753,7 @@
       </c>
       <c r="L72" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>77</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11772,18 +11774,18 @@
       </c>
       <c r="F73" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4094</v>
+        <v>4003</v>
       </c>
       <c r="H73" s="4" t="s">
         <v>308</v>
       </c>
       <c r="I73" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4276981</v>
+        <v>4063824</v>
       </c>
       <c r="L73" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>49</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11804,18 +11806,18 @@
       </c>
       <c r="F74" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4059</v>
+        <v>4003</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>309</v>
       </c>
       <c r="I74" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4803571</v>
+        <v>4708503</v>
       </c>
       <c r="L74" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>81</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11836,7 +11838,7 @@
       </c>
       <c r="F75" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4010</v>
+        <v>4039</v>
       </c>
       <c r="H75" s="4" t="s">
         <v>310</v>
@@ -11847,7 +11849,7 @@
       </c>
       <c r="L75" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11868,18 +11870,18 @@
       </c>
       <c r="F76" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4037</v>
+        <v>4007</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>311</v>
       </c>
       <c r="I76" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4407911</v>
+        <v>4054096</v>
       </c>
       <c r="L76" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>88</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11900,18 +11902,18 @@
       </c>
       <c r="F77" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4013</v>
+        <v>4025</v>
       </c>
       <c r="H77" s="4" t="s">
         <v>312</v>
       </c>
       <c r="I77" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4991192</v>
+        <v>4175000</v>
       </c>
       <c r="L77" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11932,18 +11934,18 @@
       </c>
       <c r="F78" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4002</v>
+        <v>4072</v>
       </c>
       <c r="H78" s="4" t="s">
         <v>313</v>
       </c>
       <c r="I78" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4074389</v>
+        <v>4524552</v>
       </c>
       <c r="L78" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>83</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11964,18 +11966,18 @@
       </c>
       <c r="F79" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4055</v>
+        <v>4018</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>314</v>
       </c>
       <c r="I79" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>5050000</v>
+        <v>4135184</v>
       </c>
       <c r="L79" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>29</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11996,18 +11998,18 @@
       </c>
       <c r="F80" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4092</v>
+        <v>4034</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>315</v>
       </c>
       <c r="I80" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4907375</v>
+        <v>4962673</v>
       </c>
       <c r="L80" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>36</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12028,18 +12030,18 @@
       </c>
       <c r="F81" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4015</v>
+        <v>4041</v>
       </c>
       <c r="H81" s="4" t="s">
         <v>316</v>
       </c>
       <c r="I81" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>5050000</v>
+        <v>4050512</v>
       </c>
       <c r="L81" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12060,18 +12062,18 @@
       </c>
       <c r="F82" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4062</v>
+        <v>4056</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I82" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4051331</v>
+        <v>4050512</v>
       </c>
       <c r="L82" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12092,18 +12094,18 @@
       </c>
       <c r="F83" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4011</v>
+        <v>4049</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>318</v>
       </c>
       <c r="I83" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4096656</v>
+        <v>4074389</v>
       </c>
       <c r="L83" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>24</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12124,18 +12126,18 @@
       </c>
       <c r="F84" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4065</v>
+        <v>4000</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>319</v>
       </c>
       <c r="I84" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4051000</v>
+        <v>4054096</v>
       </c>
       <c r="L84" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>61</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12156,18 +12158,18 @@
       </c>
       <c r="F85" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4072</v>
+        <v>4075</v>
       </c>
       <c r="H85" s="4" t="s">
         <v>320</v>
       </c>
       <c r="I85" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4089304</v>
+        <v>4051728</v>
       </c>
       <c r="L85" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>52</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12188,18 +12190,18 @@
       </c>
       <c r="F86" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4063</v>
+        <v>4049</v>
       </c>
       <c r="H86" s="4" t="s">
         <v>321</v>
       </c>
       <c r="I86" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4276981</v>
+        <v>4393000</v>
       </c>
       <c r="L86" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12220,18 +12222,18 @@
       </c>
       <c r="F87" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4004</v>
+        <v>4059</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>322</v>
       </c>
       <c r="I87" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4182651</v>
+        <v>4488976</v>
       </c>
       <c r="L87" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>100</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12252,18 +12254,18 @@
       </c>
       <c r="F88" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4086</v>
+        <v>4056</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>323</v>
       </c>
       <c r="I88" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4779000</v>
+        <v>4053375</v>
       </c>
       <c r="L88" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>97</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12284,18 +12286,18 @@
       </c>
       <c r="F89" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4062</v>
+        <v>4005</v>
       </c>
       <c r="H89" s="4" t="s">
         <v>324</v>
       </c>
       <c r="I89" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4100653</v>
+        <v>4129507</v>
       </c>
       <c r="L89" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>50</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12323,11 +12325,11 @@
       </c>
       <c r="I90" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4054096</v>
+        <v>4255379</v>
       </c>
       <c r="L90" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>38</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12348,18 +12350,18 @@
       </c>
       <c r="F91" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4040</v>
+        <v>4093</v>
       </c>
       <c r="H91" s="4" t="s">
         <v>326</v>
       </c>
       <c r="I91" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4054096</v>
+        <v>4991192</v>
       </c>
       <c r="L91" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12380,18 +12382,18 @@
       </c>
       <c r="F92" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4054</v>
+        <v>4047</v>
       </c>
       <c r="H92" s="4" t="s">
         <v>327</v>
       </c>
       <c r="I92" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4054096</v>
+        <v>4118921</v>
       </c>
       <c r="L92" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>68</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12412,18 +12414,18 @@
       </c>
       <c r="F93" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4024</v>
+        <v>4086</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>328</v>
       </c>
       <c r="I93" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4077000</v>
+        <v>4050343</v>
       </c>
       <c r="L93" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>29</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12444,18 +12446,18 @@
       </c>
       <c r="F94" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4086</v>
+        <v>4039</v>
       </c>
       <c r="H94" s="4" t="s">
         <v>329</v>
       </c>
       <c r="I94" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4089304</v>
+        <v>4337496</v>
       </c>
       <c r="L94" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>43</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12476,18 +12478,18 @@
       </c>
       <c r="F95" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4006</v>
+        <v>4011</v>
       </c>
       <c r="H95" s="4" t="s">
         <v>330</v>
       </c>
       <c r="I95" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4288328</v>
+        <v>4708503</v>
       </c>
       <c r="L95" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>35</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12508,18 +12510,18 @@
       </c>
       <c r="F96" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4028</v>
+        <v>4066</v>
       </c>
       <c r="H96" s="4" t="s">
         <v>331</v>
       </c>
       <c r="I96" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4060648</v>
+        <v>4053375</v>
       </c>
       <c r="L96" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>26</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12540,18 +12542,18 @@
       </c>
       <c r="F97" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4063</v>
+        <v>4045</v>
       </c>
       <c r="H97" s="4" t="s">
         <v>332</v>
       </c>
       <c r="I97" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4067576</v>
+        <v>4621787</v>
       </c>
       <c r="L97" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>23</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12572,18 +12574,18 @@
       </c>
       <c r="F98" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4093</v>
+        <v>4087</v>
       </c>
       <c r="H98" s="4" t="s">
         <v>333</v>
       </c>
       <c r="I98" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4754969</v>
+        <v>4642704</v>
       </c>
       <c r="L98" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>26</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12604,18 +12606,18 @@
       </c>
       <c r="F99" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4054</v>
+        <v>4024</v>
       </c>
       <c r="H99" s="4" t="s">
         <v>334</v>
       </c>
       <c r="I99" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4991192</v>
+        <v>4562000</v>
       </c>
       <c r="L99" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>83</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12636,18 +12638,18 @@
       </c>
       <c r="F100" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4025</v>
+        <v>4030</v>
       </c>
       <c r="H100" s="4" t="s">
         <v>335</v>
       </c>
       <c r="I100" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4063824</v>
+        <v>4160592</v>
       </c>
       <c r="L100" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>41</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12668,18 +12670,18 @@
       </c>
       <c r="F101" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4097</v>
+        <v>4003</v>
       </c>
       <c r="H101" s="4" t="s">
         <v>336</v>
       </c>
       <c r="I101" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4077000</v>
+        <v>4054096</v>
       </c>
       <c r="L101" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>100</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12700,18 +12702,18 @@
       </c>
       <c r="F102" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4060</v>
+        <v>4013</v>
       </c>
       <c r="H102" s="4" t="s">
         <v>337</v>
       </c>
       <c r="I102" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4288328</v>
+        <v>4828688</v>
       </c>
       <c r="L102" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>17</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12732,18 +12734,18 @@
       </c>
       <c r="F103" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4006</v>
+        <v>4018</v>
       </c>
       <c r="H103" s="4" t="s">
         <v>338</v>
       </c>
       <c r="I103" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4506533</v>
+        <v>4524552</v>
       </c>
       <c r="L103" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>61</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12764,18 +12766,18 @@
       </c>
       <c r="F104" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4045</v>
+        <v>4077</v>
       </c>
       <c r="H104" s="4" t="s">
         <v>339</v>
       </c>
       <c r="I104" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4581441</v>
+        <v>4543039</v>
       </c>
       <c r="L104" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12796,18 +12798,18 @@
       </c>
       <c r="F105" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4043</v>
+        <v>4097</v>
       </c>
       <c r="H105" s="4" t="s">
         <v>340</v>
       </c>
       <c r="I105" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4543039</v>
+        <v>4051331</v>
       </c>
       <c r="L105" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>65</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12828,18 +12830,18 @@
       </c>
       <c r="F106" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4012</v>
+        <v>4035</v>
       </c>
       <c r="H106" s="4" t="s">
         <v>341</v>
       </c>
       <c r="I106" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4562000</v>
+        <v>4141125</v>
       </c>
       <c r="L106" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>70</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12860,18 +12862,18 @@
       </c>
       <c r="F107" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4100</v>
+        <v>4029</v>
       </c>
       <c r="H107" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I107" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4880584</v>
+        <v>4803571</v>
       </c>
       <c r="L107" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>28</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12892,18 +12894,18 @@
       </c>
       <c r="F108" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4019</v>
+        <v>4077</v>
       </c>
       <c r="H108" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I108" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4393000</v>
+        <v>4506533</v>
       </c>
       <c r="L108" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>98</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12924,18 +12926,18 @@
       </c>
       <c r="F109" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4079</v>
+        <v>4019</v>
       </c>
       <c r="H109" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I109" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4300047</v>
+        <v>4104872</v>
       </c>
       <c r="L109" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>45</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12956,18 +12958,18 @@
       </c>
       <c r="F110" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4062</v>
+        <v>4024</v>
       </c>
       <c r="H110" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I110" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4880584</v>
+        <v>4235193</v>
       </c>
       <c r="L110" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>59</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12988,18 +12990,18 @@
       </c>
       <c r="F111" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4098</v>
+        <v>4024</v>
       </c>
       <c r="H111" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I111" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4082768</v>
+        <v>4129507</v>
       </c>
       <c r="L111" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13007,47 +13009,415 @@
       <c r="D112" s="2"/>
       <c r="E112" s="3"/>
     </row>
-    <row r="113" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B113" s="2"/>
       <c r="D113" s="2"/>
-    </row>
-    <row r="114" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E113" s="3"/>
+    </row>
+    <row r="114" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B114" s="2"/>
       <c r="D114" s="2"/>
-    </row>
-    <row r="115" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E114" s="3"/>
+    </row>
+    <row r="115" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B115" s="2"/>
       <c r="D115" s="2"/>
-    </row>
-    <row r="116" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E115" s="3"/>
+    </row>
+    <row r="116" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B116" s="2"/>
       <c r="D116" s="2"/>
-    </row>
-    <row r="117" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E116" s="3"/>
+    </row>
+    <row r="117" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B117" s="2"/>
       <c r="D117" s="2"/>
-    </row>
-    <row r="118" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E117" s="3"/>
+    </row>
+    <row r="118" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B118" s="2"/>
       <c r="D118" s="2"/>
-    </row>
-    <row r="119" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E118" s="3"/>
+    </row>
+    <row r="119" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B119" s="2"/>
       <c r="D119" s="2"/>
-    </row>
-    <row r="120" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E119" s="3"/>
+    </row>
+    <row r="120" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B120" s="2"/>
       <c r="D120" s="2"/>
-    </row>
-    <row r="121" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E120" s="3"/>
+    </row>
+    <row r="121" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B121" s="2"/>
       <c r="D121" s="2"/>
-    </row>
-    <row r="122" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E121" s="3"/>
+    </row>
+    <row r="122" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B122" s="2"/>
       <c r="D122" s="2"/>
-    </row>
-    <row r="123" spans="2:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E122" s="3"/>
+    </row>
+    <row r="123" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B123" s="2"/>
       <c r="D123" s="2"/>
+      <c r="E123" s="3"/>
+    </row>
+    <row r="124" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B124" s="2"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="3"/>
+    </row>
+    <row r="125" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B125" s="2"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="3"/>
+    </row>
+    <row r="126" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B126" s="2"/>
+      <c r="D126" s="2"/>
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B127" s="2"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="3"/>
+    </row>
+    <row r="128" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="3"/>
+    </row>
+    <row r="129" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B129" s="2"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="3"/>
+    </row>
+    <row r="130" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B130" s="2"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="3"/>
+    </row>
+    <row r="131" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B131" s="2"/>
+      <c r="D131" s="2"/>
+      <c r="E131" s="3"/>
+    </row>
+    <row r="132" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B132" s="2"/>
+      <c r="D132" s="2"/>
+      <c r="E132" s="3"/>
+    </row>
+    <row r="133" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B133" s="2"/>
+      <c r="D133" s="2"/>
+      <c r="E133" s="3"/>
+    </row>
+    <row r="134" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B134" s="2"/>
+      <c r="D134" s="2"/>
+      <c r="E134" s="3"/>
+    </row>
+    <row r="135" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B135" s="2"/>
+      <c r="D135" s="2"/>
+      <c r="E135" s="3"/>
+    </row>
+    <row r="136" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B136" s="2"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="3"/>
+    </row>
+    <row r="137" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B137" s="2"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="3"/>
+    </row>
+    <row r="138" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B138" s="2"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="3"/>
+    </row>
+    <row r="139" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B139" s="2"/>
+      <c r="D139" s="2"/>
+      <c r="E139" s="3"/>
+    </row>
+    <row r="140" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="3"/>
+    </row>
+    <row r="141" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B141" s="2"/>
+      <c r="D141" s="2"/>
+      <c r="E141" s="3"/>
+    </row>
+    <row r="142" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B142" s="2"/>
+      <c r="D142" s="2"/>
+      <c r="E142" s="3"/>
+    </row>
+    <row r="143" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B143" s="2"/>
+      <c r="D143" s="2"/>
+      <c r="E143" s="3"/>
+    </row>
+    <row r="144" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B144" s="2"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="3"/>
+    </row>
+    <row r="145" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="3"/>
+    </row>
+    <row r="146" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="3"/>
+    </row>
+    <row r="147" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B147" s="2"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="3"/>
+    </row>
+    <row r="148" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B148" s="2"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="3"/>
+    </row>
+    <row r="149" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="3"/>
+    </row>
+    <row r="150" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B150" s="2"/>
+      <c r="D150" s="2"/>
+      <c r="E150" s="3"/>
+    </row>
+    <row r="151" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B151" s="2"/>
+      <c r="D151" s="2"/>
+      <c r="E151" s="3"/>
+    </row>
+    <row r="152" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="E152" s="3"/>
+    </row>
+    <row r="153" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="3"/>
+    </row>
+    <row r="154" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B154" s="2"/>
+      <c r="D154" s="2"/>
+      <c r="E154" s="3"/>
+    </row>
+    <row r="155" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B155" s="2"/>
+      <c r="D155" s="2"/>
+      <c r="E155" s="3"/>
+    </row>
+    <row r="156" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B156" s="2"/>
+      <c r="D156" s="2"/>
+      <c r="E156" s="3"/>
+    </row>
+    <row r="157" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B157" s="2"/>
+      <c r="D157" s="2"/>
+      <c r="E157" s="3"/>
+    </row>
+    <row r="158" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="3"/>
+    </row>
+    <row r="159" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="3"/>
+    </row>
+    <row r="160" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="3"/>
+    </row>
+    <row r="161" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="3"/>
+    </row>
+    <row r="162" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B162" s="2"/>
+      <c r="D162" s="2"/>
+      <c r="E162" s="3"/>
+    </row>
+    <row r="163" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B163" s="2"/>
+      <c r="D163" s="2"/>
+      <c r="E163" s="3"/>
+    </row>
+    <row r="164" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B164" s="2"/>
+      <c r="D164" s="2"/>
+      <c r="E164" s="3"/>
+    </row>
+    <row r="165" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B165" s="2"/>
+      <c r="D165" s="2"/>
+      <c r="E165" s="3"/>
+    </row>
+    <row r="166" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B166" s="2"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="3"/>
+    </row>
+    <row r="167" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B167" s="2"/>
+      <c r="D167" s="2"/>
+      <c r="E167" s="3"/>
+    </row>
+    <row r="168" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B168" s="2"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="3"/>
+    </row>
+    <row r="169" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B169" s="2"/>
+      <c r="D169" s="2"/>
+      <c r="E169" s="3"/>
+    </row>
+    <row r="170" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B170" s="2"/>
+      <c r="D170" s="2"/>
+      <c r="E170" s="3"/>
+    </row>
+    <row r="171" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B171" s="2"/>
+      <c r="D171" s="2"/>
+      <c r="E171" s="3"/>
+    </row>
+    <row r="172" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B172" s="2"/>
+      <c r="D172" s="2"/>
+      <c r="E172" s="3"/>
+    </row>
+    <row r="173" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B173" s="2"/>
+      <c r="D173" s="2"/>
+      <c r="E173" s="3"/>
+    </row>
+    <row r="174" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B174" s="2"/>
+      <c r="D174" s="2"/>
+      <c r="E174" s="3"/>
+    </row>
+    <row r="175" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B175" s="2"/>
+      <c r="D175" s="2"/>
+      <c r="E175" s="3"/>
+    </row>
+    <row r="176" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B176" s="2"/>
+      <c r="D176" s="2"/>
+      <c r="E176" s="3"/>
+    </row>
+    <row r="177" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B177" s="2"/>
+      <c r="D177" s="2"/>
+      <c r="E177" s="3"/>
+    </row>
+    <row r="178" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B178" s="2"/>
+      <c r="D178" s="2"/>
+      <c r="E178" s="3"/>
+    </row>
+    <row r="179" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B179" s="2"/>
+      <c r="D179" s="2"/>
+      <c r="E179" s="3"/>
+    </row>
+    <row r="180" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B180" s="2"/>
+      <c r="D180" s="2"/>
+      <c r="E180" s="3"/>
+    </row>
+    <row r="181" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B181" s="2"/>
+      <c r="D181" s="2"/>
+      <c r="E181" s="3"/>
+    </row>
+    <row r="182" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B182" s="2"/>
+      <c r="D182" s="2"/>
+      <c r="E182" s="3"/>
+    </row>
+    <row r="183" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B183" s="2"/>
+      <c r="D183" s="2"/>
+      <c r="E183" s="3"/>
+    </row>
+    <row r="184" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B184" s="2"/>
+      <c r="D184" s="2"/>
+      <c r="E184" s="3"/>
+    </row>
+    <row r="185" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B185" s="2"/>
+      <c r="D185" s="2"/>
+      <c r="E185" s="3"/>
+    </row>
+    <row r="186" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B186" s="2"/>
+      <c r="D186" s="2"/>
+      <c r="E186" s="3"/>
+    </row>
+    <row r="187" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B187" s="2"/>
+      <c r="D187" s="2"/>
+      <c r="E187" s="3"/>
+    </row>
+    <row r="188" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B188" s="2"/>
+      <c r="D188" s="2"/>
+      <c r="E188" s="3"/>
+    </row>
+    <row r="189" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B189" s="2"/>
+      <c r="D189" s="2"/>
+      <c r="E189" s="3"/>
+    </row>
+    <row r="190" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B190" s="2"/>
+      <c r="D190" s="2"/>
+      <c r="E190" s="3"/>
+    </row>
+    <row r="191" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B191" s="2"/>
+      <c r="D191" s="2"/>
+      <c r="E191" s="3"/>
+    </row>
+    <row r="192" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B192" s="2"/>
+      <c r="D192" s="2"/>
+      <c r="E192" s="3"/>
+    </row>
+    <row r="193" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B193" s="2"/>
+      <c r="D193" s="2"/>
+      <c r="E193" s="3"/>
+    </row>
+    <row r="194" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B194" s="2"/>
+      <c r="D194" s="2"/>
+      <c r="E194" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -13114,7 +13484,7 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">RANDBETWEEN(1,100) + 3000</f>
-        <v>3039</v>
+        <v>3006</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -13144,7 +13514,7 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3006</v>
+        <v>3041</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -13159,7 +13529,7 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3067</v>
+        <v>3046</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -13174,7 +13544,7 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3002</v>
+        <v>3031</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -13189,7 +13559,7 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3048</v>
+        <v>3075</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -13204,7 +13574,7 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3022</v>
+        <v>3050</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -13219,7 +13589,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3058</v>
+        <v>3070</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -13234,7 +13604,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3028</v>
+        <v>3054</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -13249,7 +13619,7 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3100</v>
+        <v>3045</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -13264,7 +13634,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3062</v>
+        <v>3094</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -13279,7 +13649,7 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3025</v>
+        <v>3053</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -13294,7 +13664,7 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3007</v>
+        <v>3025</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -13309,7 +13679,7 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3049</v>
+        <v>3081</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -13324,7 +13694,7 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3044</v>
+        <v>3037</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -13339,7 +13709,7 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3089</v>
+        <v>3045</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -13354,7 +13724,7 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3011</v>
+        <v>3054</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -13369,7 +13739,7 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3077</v>
+        <v>3056</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -13384,7 +13754,7 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3020</v>
+        <v>3025</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -13399,7 +13769,7 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3070</v>
+        <v>3020</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -13414,7 +13784,7 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3093</v>
+        <v>3072</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -13429,7 +13799,7 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3022</v>
+        <v>3090</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -13444,7 +13814,7 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3038</v>
+        <v>3029</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -13459,7 +13829,7 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3078</v>
+        <v>3036</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -13474,7 +13844,7 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3095</v>
+        <v>3064</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -13489,7 +13859,7 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3056</v>
+        <v>3042</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
@@ -13504,7 +13874,7 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3042</v>
+        <v>3097</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -13519,7 +13889,7 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3028</v>
+        <v>3024</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
@@ -13534,7 +13904,7 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3058</v>
+        <v>3002</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -13549,7 +13919,7 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3051</v>
+        <v>3015</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
@@ -13564,7 +13934,7 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3012</v>
+        <v>3050</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
@@ -13579,7 +13949,7 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3018</v>
+        <v>3074</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
@@ -13594,7 +13964,7 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3022</v>
+        <v>3045</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
@@ -13609,7 +13979,7 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3057</v>
+        <v>3089</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
@@ -13624,7 +13994,7 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3039</v>
+        <v>3014</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
@@ -13639,7 +14009,7 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3026</v>
+        <v>3048</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -13654,7 +14024,7 @@
       </c>
       <c r="B38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3015</v>
+        <v>3079</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
@@ -13669,7 +14039,7 @@
       </c>
       <c r="B39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3008</v>
+        <v>3072</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
@@ -13684,7 +14054,7 @@
       </c>
       <c r="B40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3002</v>
+        <v>3100</v>
       </c>
       <c r="D40" s="1">
         <v>0</v>
@@ -13699,7 +14069,7 @@
       </c>
       <c r="B41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3081</v>
+        <v>3052</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
@@ -13714,7 +14084,7 @@
       </c>
       <c r="B42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3028</v>
+        <v>3094</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
@@ -13729,7 +14099,7 @@
       </c>
       <c r="B43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3007</v>
+        <v>3095</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
@@ -13744,7 +14114,7 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3096</v>
+        <v>3015</v>
       </c>
       <c r="D44" s="1">
         <v>0</v>
@@ -13759,7 +14129,7 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3048</v>
+        <v>3012</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
@@ -13774,7 +14144,7 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3100</v>
+        <v>3072</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
@@ -13789,7 +14159,7 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3068</v>
+        <v>3044</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
@@ -13804,7 +14174,7 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3091</v>
+        <v>3080</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
@@ -13819,7 +14189,7 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3040</v>
+        <v>3090</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
@@ -13834,7 +14204,7 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3006</v>
+        <v>3043</v>
       </c>
       <c r="D50" s="1">
         <v>0</v>
@@ -13849,7 +14219,7 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3034</v>
+        <v>3013</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
@@ -13864,7 +14234,7 @@
       </c>
       <c r="B52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3061</v>
+        <v>3087</v>
       </c>
       <c r="D52" s="1">
         <v>0</v>
@@ -13879,7 +14249,7 @@
       </c>
       <c r="B53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3004</v>
+        <v>3016</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
@@ -13894,7 +14264,7 @@
       </c>
       <c r="B54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3020</v>
+        <v>3034</v>
       </c>
       <c r="D54" s="1">
         <v>0</v>
@@ -13909,7 +14279,7 @@
       </c>
       <c r="B55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3024</v>
+        <v>3003</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -13924,7 +14294,7 @@
       </c>
       <c r="B56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3057</v>
+        <v>3052</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
@@ -13939,7 +14309,7 @@
       </c>
       <c r="B57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3027</v>
+        <v>3020</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
@@ -13954,7 +14324,7 @@
       </c>
       <c r="B58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3075</v>
+        <v>3027</v>
       </c>
       <c r="D58" s="1">
         <v>0</v>
@@ -13969,7 +14339,7 @@
       </c>
       <c r="B59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3013</v>
+        <v>3074</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
@@ -13984,7 +14354,7 @@
       </c>
       <c r="B60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3064</v>
+        <v>3040</v>
       </c>
       <c r="D60" s="1">
         <v>0</v>
@@ -13999,7 +14369,7 @@
       </c>
       <c r="B61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3033</v>
+        <v>3100</v>
       </c>
       <c r="D61" s="1">
         <v>0</v>
@@ -14014,7 +14384,7 @@
       </c>
       <c r="B62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3069</v>
+        <v>3051</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
@@ -14029,7 +14399,7 @@
       </c>
       <c r="B63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3012</v>
+        <v>3056</v>
       </c>
       <c r="D63" s="1">
         <v>0</v>
@@ -14044,7 +14414,7 @@
       </c>
       <c r="B64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3072</v>
+        <v>3067</v>
       </c>
       <c r="D64" s="1">
         <v>0</v>
@@ -14059,7 +14429,7 @@
       </c>
       <c r="B65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3061</v>
+        <v>3034</v>
       </c>
       <c r="D65" s="1">
         <v>0</v>
@@ -14074,7 +14444,7 @@
       </c>
       <c r="B66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3074</v>
+        <v>3079</v>
       </c>
       <c r="D66" s="1">
         <v>0</v>
@@ -14089,7 +14459,7 @@
       </c>
       <c r="B67" s="1">
         <f t="shared" ref="B67:B110" ca="1" si="1">RANDBETWEEN(1,100) + 3000</f>
-        <v>3032</v>
+        <v>3049</v>
       </c>
       <c r="D67" s="1">
         <v>0</v>
@@ -14104,7 +14474,7 @@
       </c>
       <c r="B68" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3077</v>
+        <v>3016</v>
       </c>
       <c r="D68" s="1">
         <v>0</v>
@@ -14119,7 +14489,7 @@
       </c>
       <c r="B69" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3092</v>
+        <v>3088</v>
       </c>
       <c r="D69" s="1">
         <v>0</v>
@@ -14134,7 +14504,7 @@
       </c>
       <c r="B70" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3076</v>
+        <v>3052</v>
       </c>
       <c r="D70" s="1">
         <v>0</v>
@@ -14149,7 +14519,7 @@
       </c>
       <c r="B71" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3035</v>
+        <v>3095</v>
       </c>
       <c r="D71" s="1">
         <v>0</v>
@@ -14164,7 +14534,7 @@
       </c>
       <c r="B72" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3072</v>
+        <v>3049</v>
       </c>
       <c r="D72" s="1">
         <v>0</v>
@@ -14179,7 +14549,7 @@
       </c>
       <c r="B73" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3018</v>
+        <v>3003</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -14194,7 +14564,7 @@
       </c>
       <c r="B74" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3088</v>
+        <v>3036</v>
       </c>
       <c r="D74" s="1">
         <v>0</v>
@@ -14209,7 +14579,7 @@
       </c>
       <c r="B75" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3073</v>
+        <v>3074</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
@@ -14224,7 +14594,7 @@
       </c>
       <c r="B76" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3047</v>
+        <v>3002</v>
       </c>
       <c r="D76" s="1">
         <v>0</v>
@@ -14239,7 +14609,7 @@
       </c>
       <c r="B77" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3016</v>
+        <v>3010</v>
       </c>
       <c r="D77" s="1">
         <v>0</v>
@@ -14254,7 +14624,7 @@
       </c>
       <c r="B78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3016</v>
+        <v>3027</v>
       </c>
       <c r="D78" s="1">
         <v>0</v>
@@ -14269,7 +14639,7 @@
       </c>
       <c r="B79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3038</v>
+        <v>3045</v>
       </c>
       <c r="D79" s="1">
         <v>0</v>
@@ -14284,7 +14654,7 @@
       </c>
       <c r="B80" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3059</v>
+        <v>3098</v>
       </c>
       <c r="D80" s="1">
         <v>0</v>
@@ -14299,7 +14669,7 @@
       </c>
       <c r="B81" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3091</v>
+        <v>3052</v>
       </c>
       <c r="D81" s="1">
         <v>0</v>
@@ -14314,7 +14684,7 @@
       </c>
       <c r="B82" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3038</v>
+        <v>3049</v>
       </c>
       <c r="D82" s="1">
         <v>0</v>
@@ -14329,7 +14699,7 @@
       </c>
       <c r="B83" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3007</v>
+        <v>3002</v>
       </c>
       <c r="D83" s="1">
         <v>0</v>
@@ -14344,7 +14714,7 @@
       </c>
       <c r="B84" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3018</v>
+        <v>3049</v>
       </c>
       <c r="D84" s="1">
         <v>0</v>
@@ -14359,7 +14729,7 @@
       </c>
       <c r="B85" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3025</v>
+        <v>3094</v>
       </c>
       <c r="D85" s="1">
         <v>0</v>
@@ -14374,7 +14744,7 @@
       </c>
       <c r="B86" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3028</v>
+        <v>3098</v>
       </c>
       <c r="D86" s="1">
         <v>0</v>
@@ -14389,7 +14759,7 @@
       </c>
       <c r="B87" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3097</v>
+        <v>3046</v>
       </c>
       <c r="D87" s="1">
         <v>0</v>
@@ -14404,7 +14774,7 @@
       </c>
       <c r="B88" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3081</v>
+        <v>3006</v>
       </c>
       <c r="D88" s="1">
         <v>0</v>
@@ -14419,7 +14789,7 @@
       </c>
       <c r="B89" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3065</v>
+        <v>3001</v>
       </c>
       <c r="D89" s="1">
         <v>0</v>
@@ -14434,7 +14804,7 @@
       </c>
       <c r="B90" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3018</v>
+        <v>3076</v>
       </c>
       <c r="D90" s="1">
         <v>0</v>
@@ -14449,7 +14819,7 @@
       </c>
       <c r="B91" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3002</v>
+        <v>3013</v>
       </c>
       <c r="D91" s="1">
         <v>0</v>
@@ -14464,7 +14834,7 @@
       </c>
       <c r="B92" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3079</v>
+        <v>3067</v>
       </c>
       <c r="D92" s="1">
         <v>0</v>
@@ -14479,7 +14849,7 @@
       </c>
       <c r="B93" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3057</v>
+        <v>3083</v>
       </c>
       <c r="D93" s="1">
         <v>0</v>
@@ -14494,7 +14864,7 @@
       </c>
       <c r="B94" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3048</v>
+        <v>3002</v>
       </c>
       <c r="D94" s="1">
         <v>0</v>
@@ -14509,7 +14879,7 @@
       </c>
       <c r="B95" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3067</v>
+        <v>3015</v>
       </c>
       <c r="D95" s="1">
         <v>0</v>
@@ -14524,7 +14894,7 @@
       </c>
       <c r="B96" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3095</v>
+        <v>3011</v>
       </c>
       <c r="D96" s="1">
         <v>0</v>
@@ -14539,7 +14909,7 @@
       </c>
       <c r="B97" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3021</v>
+        <v>3061</v>
       </c>
       <c r="D97" s="1">
         <v>0</v>
@@ -14554,7 +14924,7 @@
       </c>
       <c r="B98" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3075</v>
+        <v>3023</v>
       </c>
       <c r="D98" s="1">
         <v>0</v>
@@ -14569,7 +14939,7 @@
       </c>
       <c r="B99" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3091</v>
+        <v>3083</v>
       </c>
       <c r="D99" s="1">
         <v>0</v>
@@ -14584,7 +14954,7 @@
       </c>
       <c r="B100" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3089</v>
+        <v>3046</v>
       </c>
       <c r="D100" s="1">
         <v>0</v>
@@ -14599,7 +14969,7 @@
       </c>
       <c r="B101" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3042</v>
+        <v>3097</v>
       </c>
       <c r="D101" s="1">
         <v>0</v>
@@ -14614,7 +14984,7 @@
       </c>
       <c r="B102" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3091</v>
+        <v>3045</v>
       </c>
       <c r="D102" s="1">
         <v>0</v>
@@ -14629,7 +14999,7 @@
       </c>
       <c r="B103" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3086</v>
+        <v>3085</v>
       </c>
       <c r="D103" s="1">
         <v>0</v>
@@ -14644,7 +15014,7 @@
       </c>
       <c r="B104" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3083</v>
+        <v>3095</v>
       </c>
       <c r="D104" s="1">
         <v>0</v>
@@ -14659,7 +15029,7 @@
       </c>
       <c r="B105" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3065</v>
+        <v>3095</v>
       </c>
       <c r="D105" s="1">
         <v>0</v>
@@ -14674,7 +15044,7 @@
       </c>
       <c r="B106" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3055</v>
+        <v>3047</v>
       </c>
       <c r="D106" s="1">
         <v>0</v>
@@ -14689,7 +15059,7 @@
       </c>
       <c r="B107" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3024</v>
+        <v>3050</v>
       </c>
       <c r="D107" s="1">
         <v>0</v>
@@ -14704,7 +15074,7 @@
       </c>
       <c r="B108" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3002</v>
+        <v>3050</v>
       </c>
       <c r="D108" s="1">
         <v>0</v>
@@ -14719,7 +15089,7 @@
       </c>
       <c r="B109" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3016</v>
+        <v>3020</v>
       </c>
       <c r="D109" s="1">
         <v>0</v>
@@ -14734,7 +15104,7 @@
       </c>
       <c r="B110" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3095</v>
+        <v>3003</v>
       </c>
       <c r="D110" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
prepare populate functionality for purchase model
</commit_message>
<xml_diff>
--- a/src/seeds/files/002_MalaUva_SeedFile.xlsx
+++ b/src/seeds/files/002_MalaUva_SeedFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nama/Library/CloudStorage/Dropbox/00-WF-C/2-NAMA/ROCKTHECODE/CODE/02-deliverables/22_RTC_P13_backend-react/malauva-backend/src/seeds/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8016AC81-5222-4346-9540-FDEC04CE7746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3C6E12-2F0E-C348-9C6F-C20305615F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="25700" activeTab="1" xr2:uid="{52677FAD-7042-B148-9A25-30607DD347FB}"/>
+    <workbookView xWindow="65800" yWindow="-2000" windowWidth="20560" windowHeight="25700" activeTab="2" xr2:uid="{52677FAD-7042-B148-9A25-30607DD347FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Wines" sheetId="1" r:id="rId1"/>
@@ -5411,7 +5411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A720E99C-703D-DB41-BD15-61F7B367C044}">
   <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="L105" sqref="L105"/>
     </sheetView>
   </sheetViews>
@@ -5486,7 +5486,7 @@
       </c>
       <c r="J2" s="1">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>17</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -5519,7 +5519,7 @@
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J66" ca="1" si="0">RANDBETWEEN(0,100)</f>
-        <v>96</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -5552,7 +5552,7 @@
       </c>
       <c r="J4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -5585,7 +5585,7 @@
       </c>
       <c r="J5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -5618,7 +5618,7 @@
       </c>
       <c r="J6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -5651,7 +5651,7 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -5684,7 +5684,7 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -5717,7 +5717,7 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -5750,7 +5750,7 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -5783,7 +5783,7 @@
       </c>
       <c r="J11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -5816,7 +5816,7 @@
       </c>
       <c r="J12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -5849,7 +5849,7 @@
       </c>
       <c r="J13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -5882,7 +5882,7 @@
       </c>
       <c r="J14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -5915,7 +5915,7 @@
       </c>
       <c r="J15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -5948,7 +5948,7 @@
       </c>
       <c r="J16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -5981,7 +5981,7 @@
       </c>
       <c r="J17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -6014,7 +6014,7 @@
       </c>
       <c r="J18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -6047,7 +6047,7 @@
       </c>
       <c r="J19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -6080,7 +6080,7 @@
       </c>
       <c r="J20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -6113,7 +6113,7 @@
       </c>
       <c r="J21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -6146,7 +6146,7 @@
       </c>
       <c r="J22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -6179,7 +6179,7 @@
       </c>
       <c r="J23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -6212,7 +6212,7 @@
       </c>
       <c r="J24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -6245,7 +6245,7 @@
       </c>
       <c r="J25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -6278,7 +6278,7 @@
       </c>
       <c r="J26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -6311,7 +6311,7 @@
       </c>
       <c r="J27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -6344,7 +6344,7 @@
       </c>
       <c r="J28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -6377,7 +6377,7 @@
       </c>
       <c r="J29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -6410,7 +6410,7 @@
       </c>
       <c r="J30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -6443,7 +6443,7 @@
       </c>
       <c r="J31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -6476,7 +6476,7 @@
       </c>
       <c r="J32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -6509,7 +6509,7 @@
       </c>
       <c r="J33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="J34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -6575,7 +6575,7 @@
       </c>
       <c r="J35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -6608,7 +6608,7 @@
       </c>
       <c r="J36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -6641,7 +6641,7 @@
       </c>
       <c r="J37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -6674,7 +6674,7 @@
       </c>
       <c r="J38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -6707,7 +6707,7 @@
       </c>
       <c r="J39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -6740,7 +6740,7 @@
       </c>
       <c r="J40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="J41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -6806,7 +6806,7 @@
       </c>
       <c r="J42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -6839,7 +6839,7 @@
       </c>
       <c r="J43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -6872,7 +6872,7 @@
       </c>
       <c r="J44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -6905,7 +6905,7 @@
       </c>
       <c r="J45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="J46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -6971,7 +6971,7 @@
       </c>
       <c r="J47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -7004,7 +7004,7 @@
       </c>
       <c r="J48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -7037,7 +7037,7 @@
       </c>
       <c r="J49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -7070,7 +7070,7 @@
       </c>
       <c r="J50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -7103,7 +7103,7 @@
       </c>
       <c r="J51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -7136,7 +7136,7 @@
       </c>
       <c r="J52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -7169,7 +7169,7 @@
       </c>
       <c r="J53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -7202,7 +7202,7 @@
       </c>
       <c r="J54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -7235,7 +7235,7 @@
       </c>
       <c r="J55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -7268,7 +7268,7 @@
       </c>
       <c r="J56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -7301,7 +7301,7 @@
       </c>
       <c r="J57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -7334,7 +7334,7 @@
       </c>
       <c r="J58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -7367,7 +7367,7 @@
       </c>
       <c r="J59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -7400,7 +7400,7 @@
       </c>
       <c r="J60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -7433,7 +7433,7 @@
       </c>
       <c r="J61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -7466,7 +7466,7 @@
       </c>
       <c r="J62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -7499,7 +7499,7 @@
       </c>
       <c r="J63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -7532,7 +7532,7 @@
       </c>
       <c r="J64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -7565,7 +7565,7 @@
       </c>
       <c r="J65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -7598,7 +7598,7 @@
       </c>
       <c r="J66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -7631,7 +7631,7 @@
       </c>
       <c r="J67" s="1">
         <f t="shared" ref="J67:J120" ca="1" si="1">RANDBETWEEN(0,100)</f>
-        <v>29</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -7664,7 +7664,7 @@
       </c>
       <c r="J68" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -7697,7 +7697,7 @@
       </c>
       <c r="J69" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
@@ -7730,7 +7730,7 @@
       </c>
       <c r="J70" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -7763,7 +7763,7 @@
       </c>
       <c r="J71" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -7796,7 +7796,7 @@
       </c>
       <c r="J72" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -7829,7 +7829,7 @@
       </c>
       <c r="J73" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -7862,7 +7862,7 @@
       </c>
       <c r="J74" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -7895,7 +7895,7 @@
       </c>
       <c r="J75" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
@@ -7928,7 +7928,7 @@
       </c>
       <c r="J76" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
@@ -7961,7 +7961,7 @@
       </c>
       <c r="J77" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
@@ -7994,7 +7994,7 @@
       </c>
       <c r="J78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
@@ -8027,7 +8027,7 @@
       </c>
       <c r="J79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
@@ -8060,7 +8060,7 @@
       </c>
       <c r="J80" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -8093,7 +8093,7 @@
       </c>
       <c r="J81" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>68</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
@@ -8126,7 +8126,7 @@
       </c>
       <c r="J82" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
@@ -8159,7 +8159,7 @@
       </c>
       <c r="J83" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
@@ -8192,7 +8192,7 @@
       </c>
       <c r="J84" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
@@ -8225,7 +8225,7 @@
       </c>
       <c r="J85" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
@@ -8258,7 +8258,7 @@
       </c>
       <c r="J86" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
@@ -8291,7 +8291,7 @@
       </c>
       <c r="J87" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
@@ -8324,7 +8324,7 @@
       </c>
       <c r="J88" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>36</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
@@ -8357,7 +8357,7 @@
       </c>
       <c r="J89" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <v>44</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
@@ -8390,7 +8390,7 @@
       </c>
       <c r="J90" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
@@ -8423,7 +8423,7 @@
       </c>
       <c r="J91" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
@@ -8456,7 +8456,7 @@
       </c>
       <c r="J92" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
@@ -8489,7 +8489,7 @@
       </c>
       <c r="J93" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
@@ -8522,7 +8522,7 @@
       </c>
       <c r="J94" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
@@ -8555,7 +8555,7 @@
       </c>
       <c r="J95" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>96</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="J96" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
@@ -8621,7 +8621,7 @@
       </c>
       <c r="J97" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
@@ -8654,7 +8654,7 @@
       </c>
       <c r="J98" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
@@ -8687,7 +8687,7 @@
       </c>
       <c r="J99" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
@@ -8720,7 +8720,7 @@
       </c>
       <c r="J100" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
@@ -8753,7 +8753,7 @@
       </c>
       <c r="J101" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
@@ -8786,7 +8786,7 @@
       </c>
       <c r="J102" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
@@ -8819,7 +8819,7 @@
       </c>
       <c r="J103" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
@@ -8852,7 +8852,7 @@
       </c>
       <c r="J104" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
@@ -8885,7 +8885,7 @@
       </c>
       <c r="J105" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
@@ -8918,7 +8918,7 @@
       </c>
       <c r="J106" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>68</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
@@ -8951,7 +8951,7 @@
       </c>
       <c r="J107" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
@@ -8984,7 +8984,7 @@
       </c>
       <c r="J108" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
@@ -9017,7 +9017,7 @@
       </c>
       <c r="J109" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
@@ -9050,7 +9050,7 @@
       </c>
       <c r="J110" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>85</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
@@ -9083,7 +9083,7 @@
       </c>
       <c r="J111" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
@@ -9116,7 +9116,7 @@
       </c>
       <c r="J112" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
@@ -9149,7 +9149,7 @@
       </c>
       <c r="J113" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
@@ -9182,7 +9182,7 @@
       </c>
       <c r="J114" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>73</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
@@ -9215,7 +9215,7 @@
       </c>
       <c r="J115" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>73</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
@@ -9248,7 +9248,7 @@
       </c>
       <c r="J116" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
@@ -9281,7 +9281,7 @@
       </c>
       <c r="J117" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>96</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
@@ -9314,7 +9314,7 @@
       </c>
       <c r="J118" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
@@ -9347,7 +9347,7 @@
       </c>
       <c r="J119" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
@@ -9380,7 +9380,7 @@
       </c>
       <c r="J120" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>82</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
@@ -9426,8 +9426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F341AF76-375D-CC4F-BE34-40B60AD74311}">
   <dimension ref="A1:L194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H54" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L111"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9509,11 +9509,11 @@
       </c>
       <c r="I2" s="1">
         <f t="shared" ref="I2:I66" ca="1" si="0">RANDBETWEEN(1,100) ^ 3 + 4050000</f>
-        <v>4051728</v>
+        <v>4114000</v>
       </c>
       <c r="L2" s="1">
         <f ca="1">RANDBETWEEN(1,100) + 1000</f>
-        <v>1082</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9534,18 +9534,18 @@
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F66" ca="1" si="1">RANDBETWEEN(0,100) + 4000</f>
-        <v>4029</v>
+        <v>4078</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>238</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4067576</v>
+        <v>4581441</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L66" ca="1" si="2">RANDBETWEEN(1,100) + 1000</f>
-        <v>1100</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9566,18 +9566,18 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4006</v>
+        <v>4090</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>239</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4100653</v>
+        <v>4562000</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1056</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9598,18 +9598,18 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4021</v>
+        <v>4052</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>240</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4059261</v>
+        <v>4255379</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1001</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9630,18 +9630,18 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4091</v>
+        <v>4100</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>241</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4621787</v>
+        <v>4050064</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1040</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9662,18 +9662,18 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4018</v>
+        <v>4024</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>242</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4160592</v>
+        <v>4141125</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1059</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9694,18 +9694,18 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4076</v>
+        <v>4030</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>243</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4488976</v>
+        <v>4664125</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1015</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9726,18 +9726,18 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4095</v>
+        <v>4082</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>244</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4288328</v>
+        <v>4050729</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1023</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9758,18 +9758,18 @@
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4098</v>
+        <v>4016</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>245</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4907375</v>
+        <v>4350763</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1083</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9790,18 +9790,18 @@
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4063</v>
+        <v>4005</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>246</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4055832</v>
+        <v>4991192</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1048</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9822,18 +9822,18 @@
       </c>
       <c r="F12" s="1">
         <f ca="1">RANDBETWEEN(0,100) + 4000</f>
-        <v>4011</v>
+        <v>4030</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>247</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5050000</v>
+        <v>4245112</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1085</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9854,18 +9854,18 @@
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4018</v>
+        <v>4073</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>248</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4055832</v>
+        <v>4089304</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1093</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9886,18 +9886,18 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4002</v>
+        <v>4093</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>249</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4051331</v>
+        <v>4350763</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1014</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9918,18 +9918,18 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4019</v>
+        <v>4057</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>250</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4052197</v>
+        <v>4065625</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1057</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9950,18 +9950,18 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4012</v>
+        <v>4051</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>251</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4266000</v>
+        <v>4378509</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1052</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -9982,18 +9982,18 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4009</v>
+        <v>4058</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>252</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4063824</v>
+        <v>4854357</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1030</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10014,18 +10014,18 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4066</v>
+        <v>4087</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>253</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4378509</v>
+        <v>4300047</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1096</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10046,18 +10046,18 @@
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4045</v>
+        <v>4089</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>254</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050001</v>
+        <v>4074389</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1040</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10078,18 +10078,18 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4029</v>
+        <v>4050</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>255</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4378509</v>
+        <v>4135184</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1030</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10110,18 +10110,18 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4065</v>
+        <v>4061</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>256</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4141125</v>
+        <v>4175000</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1005</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10142,18 +10142,18 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4027</v>
+        <v>4063</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>257</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4190608</v>
+        <v>4880584</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1077</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10174,18 +10174,18 @@
       </c>
       <c r="F23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4072</v>
+        <v>4100</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>258</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4562000</v>
+        <v>4050064</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1020</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10206,18 +10206,18 @@
       </c>
       <c r="F24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4088</v>
+        <v>4095</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>259</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050027</v>
+        <v>4096656</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1086</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10238,18 +10238,18 @@
       </c>
       <c r="F25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4084</v>
+        <v>4049</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>260</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4337496</v>
+        <v>4129507</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1021</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10277,11 +10277,11 @@
       </c>
       <c r="I26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4104872</v>
+        <v>4092875</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1067</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10302,18 +10302,18 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4063</v>
+        <v>4062</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>262</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4324625</v>
+        <v>4109319</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1049</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10334,18 +10334,18 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4085</v>
+        <v>4097</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>263</v>
       </c>
       <c r="I28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4153823</v>
+        <v>4854357</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1093</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10366,18 +10366,18 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4018</v>
+        <v>4030</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>264</v>
       </c>
       <c r="I29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4052197</v>
+        <v>4054913</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1029</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10398,18 +10398,18 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4001</v>
+        <v>4091</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>265</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4880584</v>
+        <v>4423248</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1096</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10430,18 +10430,18 @@
       </c>
       <c r="F31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4006</v>
+        <v>4039</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>266</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4393000</v>
+        <v>4350763</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1061</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10462,18 +10462,18 @@
       </c>
       <c r="F32" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4012</v>
+        <v>4023</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>267</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4051000</v>
+        <v>4129507</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1036</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10494,18 +10494,18 @@
       </c>
       <c r="F33" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4098</v>
+        <v>4061</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>268</v>
       </c>
       <c r="I33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4051728</v>
+        <v>4378509</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1067</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10526,18 +10526,18 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4099</v>
+        <v>4002</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>269</v>
       </c>
       <c r="I34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4581441</v>
+        <v>4488976</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1068</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10558,18 +10558,18 @@
       </c>
       <c r="F35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4027</v>
+        <v>4050</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>270</v>
       </c>
       <c r="I35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4300047</v>
+        <v>4153823</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1079</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10590,18 +10590,18 @@
       </c>
       <c r="F36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4025</v>
+        <v>4066</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>271</v>
       </c>
       <c r="I36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4153823</v>
+        <v>4077000</v>
       </c>
       <c r="L36" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1065</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10622,18 +10622,18 @@
       </c>
       <c r="F37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4090</v>
+        <v>4085</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>272</v>
       </c>
       <c r="I37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050064</v>
+        <v>4245112</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1026</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10654,18 +10654,18 @@
       </c>
       <c r="F38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4010</v>
+        <v>4096</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>273</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4664125</v>
+        <v>4488976</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1070</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10686,18 +10686,18 @@
       </c>
       <c r="F39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4031</v>
+        <v>4028</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>274</v>
       </c>
       <c r="I39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4216375</v>
+        <v>4266000</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1090</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10718,18 +10718,18 @@
       </c>
       <c r="F40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4085</v>
+        <v>4094</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>275</v>
       </c>
       <c r="I40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4225616</v>
+        <v>4052197</v>
       </c>
       <c r="L40" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1022</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10750,18 +10750,18 @@
       </c>
       <c r="F41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4096</v>
+        <v>4007</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>276</v>
       </c>
       <c r="I41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4543039</v>
+        <v>4124088</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1090</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10782,18 +10782,18 @@
       </c>
       <c r="F42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4076</v>
+        <v>4096</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>277</v>
       </c>
       <c r="I42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4129507</v>
+        <v>4063824</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1081</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10814,18 +10814,18 @@
       </c>
       <c r="F43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4068</v>
+        <v>4003</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>278</v>
       </c>
       <c r="I43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4324625</v>
+        <v>4051000</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1066</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10846,18 +10846,18 @@
       </c>
       <c r="F44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4012</v>
+        <v>4057</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>279</v>
       </c>
       <c r="I44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4055832</v>
+        <v>4124088</v>
       </c>
       <c r="L44" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1062</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10878,18 +10878,18 @@
       </c>
       <c r="F45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4062</v>
+        <v>4056</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>280</v>
       </c>
       <c r="I45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4962673</v>
+        <v>4276981</v>
       </c>
       <c r="L45" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1012</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10910,18 +10910,18 @@
       </c>
       <c r="F46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4058</v>
+        <v>4027</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>281</v>
       </c>
       <c r="I46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4907375</v>
+        <v>4153823</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1039</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10942,18 +10942,18 @@
       </c>
       <c r="F47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4008</v>
+        <v>4063</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>282</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4160592</v>
+        <v>4686056</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1091</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10974,18 +10974,18 @@
       </c>
       <c r="F48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4035</v>
+        <v>4087</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>283</v>
       </c>
       <c r="I48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4082768</v>
+        <v>4050729</v>
       </c>
       <c r="L48" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1009</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11006,18 +11006,18 @@
       </c>
       <c r="F49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4028</v>
+        <v>4096</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>284</v>
       </c>
       <c r="I49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4288328</v>
+        <v>4731472</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1042</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11038,18 +11038,18 @@
       </c>
       <c r="F50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4005</v>
+        <v>4032</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>285</v>
       </c>
       <c r="I50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4190608</v>
+        <v>4350763</v>
       </c>
       <c r="L50" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1005</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11070,18 +11070,18 @@
       </c>
       <c r="F51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4071</v>
+        <v>4073</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>286</v>
       </c>
       <c r="I51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4276981</v>
+        <v>4207464</v>
       </c>
       <c r="L51" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1056</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11102,18 +11102,18 @@
       </c>
       <c r="F52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4082</v>
+        <v>4051</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4562000</v>
+        <v>5020299</v>
       </c>
       <c r="L52" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1032</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11134,18 +11134,18 @@
       </c>
       <c r="F53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4025</v>
+        <v>4077</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>288</v>
       </c>
       <c r="I53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4216375</v>
+        <v>4053375</v>
       </c>
       <c r="L53" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1082</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11166,18 +11166,18 @@
       </c>
       <c r="F54" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4090</v>
+        <v>4040</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>289</v>
       </c>
       <c r="I54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4779000</v>
+        <v>4225616</v>
       </c>
       <c r="L54" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1069</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11198,18 +11198,18 @@
       </c>
       <c r="F55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4081</v>
+        <v>4097</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>290</v>
       </c>
       <c r="I55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4276981</v>
+        <v>4052744</v>
       </c>
       <c r="L55" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1002</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11230,18 +11230,18 @@
       </c>
       <c r="F56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4086</v>
+        <v>4052</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>291</v>
       </c>
       <c r="I56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4053375</v>
+        <v>4167649</v>
       </c>
       <c r="L56" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1082</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11262,18 +11262,18 @@
       </c>
       <c r="F57" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4005</v>
+        <v>4004</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>292</v>
       </c>
       <c r="I57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4393000</v>
+        <v>4052744</v>
       </c>
       <c r="L57" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1037</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11294,18 +11294,18 @@
       </c>
       <c r="F58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4006</v>
+        <v>4045</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>293</v>
       </c>
       <c r="I58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4378509</v>
+        <v>4051728</v>
       </c>
       <c r="L58" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1094</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11326,18 +11326,18 @@
       </c>
       <c r="F59" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4016</v>
+        <v>4098</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>294</v>
       </c>
       <c r="I59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4423248</v>
+        <v>4051000</v>
       </c>
       <c r="L59" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1065</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11358,18 +11358,18 @@
       </c>
       <c r="F60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4001</v>
+        <v>4100</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>295</v>
       </c>
       <c r="I60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4803571</v>
+        <v>4062167</v>
       </c>
       <c r="L60" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1006</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11390,18 +11390,18 @@
       </c>
       <c r="F61" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4060</v>
+        <v>4099</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>296</v>
       </c>
       <c r="I61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4089304</v>
+        <v>4488976</v>
       </c>
       <c r="L61" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1025</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11422,18 +11422,18 @@
       </c>
       <c r="F62" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4098</v>
+        <v>4081</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>297</v>
       </c>
       <c r="I62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4524552</v>
+        <v>4207464</v>
       </c>
       <c r="L62" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1064</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11454,18 +11454,18 @@
       </c>
       <c r="F63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4053</v>
+        <v>4018</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>298</v>
       </c>
       <c r="I63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050216</v>
+        <v>5050000</v>
       </c>
       <c r="L63" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1056</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11486,18 +11486,18 @@
       </c>
       <c r="F64" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4087</v>
+        <v>4092</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>299</v>
       </c>
       <c r="I64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050125</v>
+        <v>4058000</v>
       </c>
       <c r="L64" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1023</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11518,18 +11518,18 @@
       </c>
       <c r="F65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4027</v>
+        <v>4005</v>
       </c>
       <c r="H65" s="4" t="s">
         <v>300</v>
       </c>
       <c r="I65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4803571</v>
+        <v>4255379</v>
       </c>
       <c r="L65" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1012</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11550,18 +11550,18 @@
       </c>
       <c r="F66" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4060</v>
+        <v>4018</v>
       </c>
       <c r="H66" s="4" t="s">
         <v>301</v>
       </c>
       <c r="I66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4350763</v>
+        <v>4051728</v>
       </c>
       <c r="L66" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1021</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11582,18 +11582,18 @@
       </c>
       <c r="F67" s="1">
         <f t="shared" ref="F67:F111" ca="1" si="3">RANDBETWEEN(0,100) + 4000</f>
-        <v>4044</v>
+        <v>4099</v>
       </c>
       <c r="H67" s="4" t="s">
         <v>302</v>
       </c>
       <c r="I67" s="1">
         <f t="shared" ref="I67:I111" ca="1" si="4">RANDBETWEEN(1,100) ^ 3 + 4050000</f>
-        <v>4581441</v>
+        <v>4190608</v>
       </c>
       <c r="L67" s="1">
         <f t="shared" ref="L67:L111" ca="1" si="5">RANDBETWEEN(1,100) + 1000</f>
-        <v>1090</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11614,18 +11614,18 @@
       </c>
       <c r="F68" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4041</v>
+        <v>4045</v>
       </c>
       <c r="H68" s="4" t="s">
         <v>303</v>
       </c>
       <c r="I68" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4124088</v>
+        <v>4052744</v>
       </c>
       <c r="L68" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1054</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11646,18 +11646,18 @@
       </c>
       <c r="F69" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4000</v>
+        <v>4097</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>304</v>
       </c>
       <c r="I69" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4054913</v>
+        <v>4337496</v>
       </c>
       <c r="L69" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1012</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11678,18 +11678,18 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4075</v>
+        <v>4009</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>305</v>
       </c>
       <c r="I70" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4439017</v>
+        <v>5020299</v>
       </c>
       <c r="L70" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11710,18 +11710,18 @@
       </c>
       <c r="F71" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4092</v>
+        <v>4078</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>306</v>
       </c>
       <c r="I71" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4089304</v>
+        <v>4276981</v>
       </c>
       <c r="L71" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1062</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11742,18 +11742,18 @@
       </c>
       <c r="F72" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4013</v>
+        <v>4067</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>307</v>
       </c>
       <c r="I72" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4050125</v>
+        <v>4779000</v>
       </c>
       <c r="L72" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1003</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11774,18 +11774,18 @@
       </c>
       <c r="F73" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4003</v>
+        <v>4030</v>
       </c>
       <c r="H73" s="4" t="s">
         <v>308</v>
       </c>
       <c r="I73" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4063824</v>
+        <v>4324625</v>
       </c>
       <c r="L73" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1051</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11806,18 +11806,18 @@
       </c>
       <c r="F74" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4003</v>
+        <v>4061</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>309</v>
       </c>
       <c r="I74" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4708503</v>
+        <v>4074389</v>
       </c>
       <c r="L74" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1005</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11838,18 +11838,18 @@
       </c>
       <c r="F75" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4039</v>
+        <v>4012</v>
       </c>
       <c r="H75" s="4" t="s">
         <v>310</v>
       </c>
       <c r="I75" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4129507</v>
+        <v>4082768</v>
       </c>
       <c r="L75" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1098</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11870,18 +11870,18 @@
       </c>
       <c r="F76" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4007</v>
+        <v>4087</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>311</v>
       </c>
       <c r="I76" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4054096</v>
+        <v>4407911</v>
       </c>
       <c r="L76" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1099</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11902,18 +11902,18 @@
       </c>
       <c r="F77" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4025</v>
+        <v>4088</v>
       </c>
       <c r="H77" s="4" t="s">
         <v>312</v>
       </c>
       <c r="I77" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4175000</v>
+        <v>4581441</v>
       </c>
       <c r="L77" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1019</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11934,18 +11934,18 @@
       </c>
       <c r="F78" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4072</v>
+        <v>4069</v>
       </c>
       <c r="H78" s="4" t="s">
         <v>313</v>
       </c>
       <c r="I78" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4524552</v>
+        <v>4543039</v>
       </c>
       <c r="L78" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1027</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11966,18 +11966,18 @@
       </c>
       <c r="F79" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4018</v>
+        <v>4091</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>314</v>
       </c>
       <c r="I79" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4135184</v>
+        <v>4642704</v>
       </c>
       <c r="L79" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1034</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11998,18 +11998,18 @@
       </c>
       <c r="F80" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4034</v>
+        <v>4044</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>315</v>
       </c>
       <c r="I80" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4962673</v>
+        <v>4052197</v>
       </c>
       <c r="L80" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1041</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12030,18 +12030,18 @@
       </c>
       <c r="F81" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4041</v>
+        <v>4029</v>
       </c>
       <c r="H81" s="4" t="s">
         <v>316</v>
       </c>
       <c r="I81" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4050512</v>
+        <v>4062167</v>
       </c>
       <c r="L81" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1024</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12062,18 +12062,18 @@
       </c>
       <c r="F82" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4056</v>
+        <v>4046</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I82" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4050512</v>
+        <v>4664125</v>
       </c>
       <c r="L82" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1009</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12094,18 +12094,18 @@
       </c>
       <c r="F83" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4049</v>
+        <v>4024</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>318</v>
       </c>
       <c r="I83" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4074389</v>
+        <v>4880584</v>
       </c>
       <c r="L83" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1041</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12133,11 +12133,11 @@
       </c>
       <c r="I84" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4054096</v>
+        <v>4167649</v>
       </c>
       <c r="L84" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1076</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12158,18 +12158,18 @@
       </c>
       <c r="F85" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4075</v>
+        <v>4083</v>
       </c>
       <c r="H85" s="4" t="s">
         <v>320</v>
       </c>
       <c r="I85" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4051728</v>
+        <v>4962673</v>
       </c>
       <c r="L85" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1025</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12190,18 +12190,18 @@
       </c>
       <c r="F86" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4049</v>
+        <v>4032</v>
       </c>
       <c r="H86" s="4" t="s">
         <v>321</v>
       </c>
       <c r="I86" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4393000</v>
+        <v>4054913</v>
       </c>
       <c r="L86" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1093</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12229,11 +12229,11 @@
       </c>
       <c r="I87" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4488976</v>
+        <v>4182651</v>
       </c>
       <c r="L87" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1011</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12254,18 +12254,18 @@
       </c>
       <c r="F88" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4056</v>
+        <v>4021</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>323</v>
       </c>
       <c r="I88" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4053375</v>
+        <v>4207464</v>
       </c>
       <c r="L88" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1063</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12286,18 +12286,18 @@
       </c>
       <c r="F89" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4005</v>
+        <v>4077</v>
       </c>
       <c r="H89" s="4" t="s">
         <v>324</v>
       </c>
       <c r="I89" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4129507</v>
+        <v>4141125</v>
       </c>
       <c r="L89" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1010</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12318,18 +12318,18 @@
       </c>
       <c r="F90" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4039</v>
+        <v>4064</v>
       </c>
       <c r="H90" s="4" t="s">
         <v>325</v>
       </c>
       <c r="I90" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4255379</v>
+        <v>4054913</v>
       </c>
       <c r="L90" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1010</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12350,18 +12350,18 @@
       </c>
       <c r="F91" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4093</v>
+        <v>4000</v>
       </c>
       <c r="H91" s="4" t="s">
         <v>326</v>
       </c>
       <c r="I91" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4991192</v>
+        <v>4074389</v>
       </c>
       <c r="L91" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1012</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12382,18 +12382,18 @@
       </c>
       <c r="F92" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4047</v>
+        <v>4071</v>
       </c>
       <c r="H92" s="4" t="s">
         <v>327</v>
       </c>
       <c r="I92" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4118921</v>
+        <v>4051331</v>
       </c>
       <c r="L92" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1097</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12414,18 +12414,18 @@
       </c>
       <c r="F93" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4086</v>
+        <v>4054</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>328</v>
       </c>
       <c r="I93" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4050343</v>
+        <v>4854357</v>
       </c>
       <c r="L93" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1063</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12446,18 +12446,18 @@
       </c>
       <c r="F94" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4039</v>
+        <v>4100</v>
       </c>
       <c r="H94" s="4" t="s">
         <v>329</v>
       </c>
       <c r="I94" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4337496</v>
+        <v>4708503</v>
       </c>
       <c r="L94" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1059</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12478,18 +12478,18 @@
       </c>
       <c r="F95" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4011</v>
+        <v>4064</v>
       </c>
       <c r="H95" s="4" t="s">
         <v>330</v>
       </c>
       <c r="I95" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4708503</v>
+        <v>4506533</v>
       </c>
       <c r="L95" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1053</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12510,18 +12510,18 @@
       </c>
       <c r="F96" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4066</v>
+        <v>4062</v>
       </c>
       <c r="H96" s="4" t="s">
         <v>331</v>
       </c>
       <c r="I96" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4053375</v>
+        <v>4079791</v>
       </c>
       <c r="L96" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1057</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12542,18 +12542,18 @@
       </c>
       <c r="F97" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4045</v>
+        <v>4000</v>
       </c>
       <c r="H97" s="4" t="s">
         <v>332</v>
       </c>
       <c r="I97" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4621787</v>
+        <v>4455224</v>
       </c>
       <c r="L97" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1042</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12574,18 +12574,18 @@
       </c>
       <c r="F98" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4087</v>
+        <v>4082</v>
       </c>
       <c r="H98" s="4" t="s">
         <v>333</v>
       </c>
       <c r="I98" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4642704</v>
+        <v>4077000</v>
       </c>
       <c r="L98" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1016</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12606,18 +12606,18 @@
       </c>
       <c r="F99" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4024</v>
+        <v>4025</v>
       </c>
       <c r="H99" s="4" t="s">
         <v>334</v>
       </c>
       <c r="I99" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4562000</v>
+        <v>4079791</v>
       </c>
       <c r="L99" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1041</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12638,18 +12638,18 @@
       </c>
       <c r="F100" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4030</v>
+        <v>4073</v>
       </c>
       <c r="H100" s="4" t="s">
         <v>335</v>
       </c>
       <c r="I100" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4160592</v>
+        <v>4423248</v>
       </c>
       <c r="L100" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1037</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12670,18 +12670,18 @@
       </c>
       <c r="F101" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4003</v>
+        <v>4088</v>
       </c>
       <c r="H101" s="4" t="s">
         <v>336</v>
       </c>
       <c r="I101" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4054096</v>
+        <v>4052744</v>
       </c>
       <c r="L101" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1065</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12702,18 +12702,18 @@
       </c>
       <c r="F102" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4013</v>
+        <v>4052</v>
       </c>
       <c r="H102" s="4" t="s">
         <v>337</v>
       </c>
       <c r="I102" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4828688</v>
+        <v>4312144</v>
       </c>
       <c r="L102" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1009</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12734,18 +12734,18 @@
       </c>
       <c r="F103" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4018</v>
+        <v>4015</v>
       </c>
       <c r="H103" s="4" t="s">
         <v>338</v>
       </c>
       <c r="I103" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4524552</v>
+        <v>4067576</v>
       </c>
       <c r="L103" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1050</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12766,18 +12766,18 @@
       </c>
       <c r="F104" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4077</v>
+        <v>4045</v>
       </c>
       <c r="H104" s="4" t="s">
         <v>339</v>
       </c>
       <c r="I104" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4543039</v>
+        <v>4266000</v>
       </c>
       <c r="L104" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1093</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12798,18 +12798,18 @@
       </c>
       <c r="F105" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4097</v>
+        <v>4013</v>
       </c>
       <c r="H105" s="4" t="s">
         <v>340</v>
       </c>
       <c r="I105" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4051331</v>
+        <v>4067576</v>
       </c>
       <c r="L105" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1077</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12830,18 +12830,18 @@
       </c>
       <c r="F106" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4035</v>
+        <v>4001</v>
       </c>
       <c r="H106" s="4" t="s">
         <v>341</v>
       </c>
       <c r="I106" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4141125</v>
+        <v>4255379</v>
       </c>
       <c r="L106" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1080</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12862,18 +12862,18 @@
       </c>
       <c r="F107" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4029</v>
+        <v>4024</v>
       </c>
       <c r="H107" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I107" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4803571</v>
+        <v>4621787</v>
       </c>
       <c r="L107" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1031</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12894,18 +12894,18 @@
       </c>
       <c r="F108" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4077</v>
+        <v>4093</v>
       </c>
       <c r="H108" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I108" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4506533</v>
+        <v>4050064</v>
       </c>
       <c r="L108" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1062</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12926,18 +12926,18 @@
       </c>
       <c r="F109" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4019</v>
+        <v>4058</v>
       </c>
       <c r="H109" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I109" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4104872</v>
+        <v>4065625</v>
       </c>
       <c r="L109" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1088</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12958,18 +12958,18 @@
       </c>
       <c r="F110" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4024</v>
+        <v>4022</v>
       </c>
       <c r="H110" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I110" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4235193</v>
+        <v>4642704</v>
       </c>
       <c r="L110" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1094</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12990,18 +12990,18 @@
       </c>
       <c r="F111" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4024</v>
+        <v>4053</v>
       </c>
       <c r="H111" s="4" t="s">
         <v>317</v>
       </c>
       <c r="I111" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4129507</v>
+        <v>4962673</v>
       </c>
       <c r="L111" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1027</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13437,8 +13437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457D69DA-3C5E-F74C-8219-2AB83CD0093A}">
   <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13484,7 +13484,10 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">RANDBETWEEN(1,100) + 3000</f>
-        <v>3006</v>
+        <v>3093</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1001</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -13499,7 +13502,10 @@
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B66" ca="1" si="0">RANDBETWEEN(1,100) + 3000</f>
-        <v>3005</v>
+        <v>3045</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1002</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -13514,7 +13520,10 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3041</v>
+        <v>3018</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1003</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -13529,7 +13538,10 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3046</v>
+        <v>3070</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1004</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -13544,7 +13556,10 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3031</v>
+        <v>3040</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1005</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -13559,7 +13574,10 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3075</v>
+        <v>3090</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1006</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -13574,7 +13592,10 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3050</v>
+        <v>3027</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1007</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -13589,7 +13610,10 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3070</v>
+        <v>3025</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1008</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -13604,7 +13628,10 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3054</v>
+        <v>3020</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1009</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -13619,7 +13646,10 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3045</v>
+        <v>3034</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1010</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -13634,7 +13664,10 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3094</v>
+        <v>3086</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1011</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -13649,7 +13682,10 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3053</v>
+        <v>3087</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1012</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -13664,7 +13700,10 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3025</v>
+        <v>3085</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1013</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -13679,7 +13718,10 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3081</v>
+        <v>3100</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1014</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -13694,7 +13736,10 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3037</v>
+        <v>3072</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1015</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -13709,7 +13754,10 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3045</v>
+        <v>3095</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1016</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -13724,7 +13772,10 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3054</v>
+        <v>3089</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1017</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -13739,7 +13790,10 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3056</v>
+        <v>3030</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1018</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -13754,7 +13808,10 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3025</v>
+        <v>3028</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1019</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -13769,7 +13826,10 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3020</v>
+        <v>3030</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1020</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -13784,7 +13844,10 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3072</v>
+        <v>3076</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1021</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -13799,7 +13862,10 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3090</v>
+        <v>3002</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1022</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -13814,7 +13880,10 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3029</v>
+        <v>3050</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1023</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -13829,7 +13898,10 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3036</v>
+        <v>3029</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1024</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -13844,7 +13916,10 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3064</v>
+        <v>3084</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1025</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -13859,7 +13934,10 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3042</v>
+        <v>3038</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1026</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
@@ -13874,7 +13952,10 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3097</v>
+        <v>3008</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1027</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -13889,7 +13970,10 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3024</v>
+        <v>3050</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1028</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
@@ -13904,7 +13988,10 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3002</v>
+        <v>3096</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1029</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -13919,7 +14006,10 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3015</v>
+        <v>3026</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1030</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
@@ -13934,7 +14024,10 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3050</v>
+        <v>3083</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1031</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
@@ -13949,7 +14042,10 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3074</v>
+        <v>3012</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1032</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
@@ -13964,7 +14060,10 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3045</v>
+        <v>3058</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1033</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
@@ -13979,7 +14078,10 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3089</v>
+        <v>3087</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1034</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
@@ -13994,7 +14096,10 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3014</v>
+        <v>3059</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1035</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
@@ -14009,7 +14114,10 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3048</v>
+        <v>3057</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1036</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -14024,7 +14132,10 @@
       </c>
       <c r="B38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3079</v>
+        <v>3063</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1037</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
@@ -14039,7 +14150,10 @@
       </c>
       <c r="B39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3072</v>
+        <v>3061</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1038</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
@@ -14054,7 +14168,10 @@
       </c>
       <c r="B40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3100</v>
+        <v>3025</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1039</v>
       </c>
       <c r="D40" s="1">
         <v>0</v>
@@ -14069,7 +14186,10 @@
       </c>
       <c r="B41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3052</v>
+        <v>3041</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1040</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
@@ -14084,7 +14204,10 @@
       </c>
       <c r="B42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3094</v>
+        <v>3049</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1041</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
@@ -14099,7 +14222,10 @@
       </c>
       <c r="B43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3095</v>
+        <v>3073</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1042</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
@@ -14114,7 +14240,10 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3015</v>
+        <v>3020</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1043</v>
       </c>
       <c r="D44" s="1">
         <v>0</v>
@@ -14129,7 +14258,10 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3012</v>
+        <v>3014</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1044</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
@@ -14144,7 +14276,10 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3072</v>
+        <v>3061</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1045</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
@@ -14159,7 +14294,10 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3044</v>
+        <v>3034</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1046</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
@@ -14174,7 +14312,10 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3080</v>
+        <v>3033</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1047</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
@@ -14189,7 +14330,10 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3090</v>
+        <v>3021</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1048</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
@@ -14204,7 +14348,10 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3043</v>
+        <v>3057</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1049</v>
       </c>
       <c r="D50" s="1">
         <v>0</v>
@@ -14219,7 +14366,10 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3013</v>
+        <v>3009</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1050</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
@@ -14234,7 +14384,10 @@
       </c>
       <c r="B52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3087</v>
+        <v>3001</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1051</v>
       </c>
       <c r="D52" s="1">
         <v>0</v>
@@ -14249,7 +14402,10 @@
       </c>
       <c r="B53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3016</v>
+        <v>3049</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1052</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
@@ -14264,7 +14420,10 @@
       </c>
       <c r="B54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3034</v>
+        <v>3083</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1053</v>
       </c>
       <c r="D54" s="1">
         <v>0</v>
@@ -14279,7 +14438,10 @@
       </c>
       <c r="B55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3003</v>
+        <v>3036</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1054</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -14294,7 +14456,10 @@
       </c>
       <c r="B56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3052</v>
+        <v>3042</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1055</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
@@ -14309,7 +14474,10 @@
       </c>
       <c r="B57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3020</v>
+        <v>3005</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1056</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
@@ -14324,7 +14492,10 @@
       </c>
       <c r="B58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3027</v>
+        <v>3002</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1057</v>
       </c>
       <c r="D58" s="1">
         <v>0</v>
@@ -14339,7 +14510,10 @@
       </c>
       <c r="B59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3074</v>
+        <v>3056</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1058</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
@@ -14354,7 +14528,10 @@
       </c>
       <c r="B60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3040</v>
+        <v>3029</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1059</v>
       </c>
       <c r="D60" s="1">
         <v>0</v>
@@ -14369,7 +14546,10 @@
       </c>
       <c r="B61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3100</v>
+        <v>3063</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1060</v>
       </c>
       <c r="D61" s="1">
         <v>0</v>
@@ -14384,7 +14564,10 @@
       </c>
       <c r="B62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3051</v>
+        <v>3086</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1061</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
@@ -14399,7 +14582,10 @@
       </c>
       <c r="B63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3056</v>
+        <v>3068</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1062</v>
       </c>
       <c r="D63" s="1">
         <v>0</v>
@@ -14414,7 +14600,10 @@
       </c>
       <c r="B64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3067</v>
+        <v>3018</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1063</v>
       </c>
       <c r="D64" s="1">
         <v>0</v>
@@ -14429,7 +14618,10 @@
       </c>
       <c r="B65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3034</v>
+        <v>3063</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1064</v>
       </c>
       <c r="D65" s="1">
         <v>0</v>
@@ -14444,7 +14636,10 @@
       </c>
       <c r="B66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3079</v>
+        <v>3099</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1065</v>
       </c>
       <c r="D66" s="1">
         <v>0</v>
@@ -14459,7 +14654,10 @@
       </c>
       <c r="B67" s="1">
         <f t="shared" ref="B67:B110" ca="1" si="1">RANDBETWEEN(1,100) + 3000</f>
-        <v>3049</v>
+        <v>3003</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1066</v>
       </c>
       <c r="D67" s="1">
         <v>0</v>
@@ -14474,7 +14672,10 @@
       </c>
       <c r="B68" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3016</v>
+        <v>3065</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1067</v>
       </c>
       <c r="D68" s="1">
         <v>0</v>
@@ -14489,7 +14690,10 @@
       </c>
       <c r="B69" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3088</v>
+        <v>3062</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1068</v>
       </c>
       <c r="D69" s="1">
         <v>0</v>
@@ -14504,7 +14708,10 @@
       </c>
       <c r="B70" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3052</v>
+        <v>3004</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1069</v>
       </c>
       <c r="D70" s="1">
         <v>0</v>
@@ -14519,7 +14726,10 @@
       </c>
       <c r="B71" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3095</v>
+        <v>3052</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1070</v>
       </c>
       <c r="D71" s="1">
         <v>0</v>
@@ -14534,7 +14744,10 @@
       </c>
       <c r="B72" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3049</v>
+        <v>3033</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1071</v>
       </c>
       <c r="D72" s="1">
         <v>0</v>
@@ -14549,7 +14762,10 @@
       </c>
       <c r="B73" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3003</v>
+        <v>3063</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1072</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -14564,7 +14780,10 @@
       </c>
       <c r="B74" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3036</v>
+        <v>3024</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1073</v>
       </c>
       <c r="D74" s="1">
         <v>0</v>
@@ -14579,7 +14798,10 @@
       </c>
       <c r="B75" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3074</v>
+        <v>3018</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1074</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
@@ -14594,7 +14816,10 @@
       </c>
       <c r="B76" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3002</v>
+        <v>3007</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1075</v>
       </c>
       <c r="D76" s="1">
         <v>0</v>
@@ -14609,7 +14834,10 @@
       </c>
       <c r="B77" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3010</v>
+        <v>3027</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1076</v>
       </c>
       <c r="D77" s="1">
         <v>0</v>
@@ -14624,7 +14852,10 @@
       </c>
       <c r="B78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3027</v>
+        <v>3007</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1077</v>
       </c>
       <c r="D78" s="1">
         <v>0</v>
@@ -14639,7 +14870,10 @@
       </c>
       <c r="B79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3045</v>
+        <v>3091</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1078</v>
       </c>
       <c r="D79" s="1">
         <v>0</v>
@@ -14654,7 +14888,10 @@
       </c>
       <c r="B80" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3098</v>
+        <v>3089</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1079</v>
       </c>
       <c r="D80" s="1">
         <v>0</v>
@@ -14669,7 +14906,10 @@
       </c>
       <c r="B81" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3052</v>
+        <v>3059</v>
+      </c>
+      <c r="C81" s="1">
+        <v>1080</v>
       </c>
       <c r="D81" s="1">
         <v>0</v>
@@ -14684,7 +14924,10 @@
       </c>
       <c r="B82" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3049</v>
+        <v>3099</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1081</v>
       </c>
       <c r="D82" s="1">
         <v>0</v>
@@ -14699,7 +14942,10 @@
       </c>
       <c r="B83" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3002</v>
+        <v>3021</v>
+      </c>
+      <c r="C83" s="1">
+        <v>1082</v>
       </c>
       <c r="D83" s="1">
         <v>0</v>
@@ -14714,7 +14960,10 @@
       </c>
       <c r="B84" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3049</v>
+        <v>3076</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1083</v>
       </c>
       <c r="D84" s="1">
         <v>0</v>
@@ -14729,7 +14978,10 @@
       </c>
       <c r="B85" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3094</v>
+        <v>3052</v>
+      </c>
+      <c r="C85" s="1">
+        <v>1084</v>
       </c>
       <c r="D85" s="1">
         <v>0</v>
@@ -14744,7 +14996,10 @@
       </c>
       <c r="B86" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3098</v>
+        <v>3044</v>
+      </c>
+      <c r="C86" s="1">
+        <v>1085</v>
       </c>
       <c r="D86" s="1">
         <v>0</v>
@@ -14759,7 +15014,10 @@
       </c>
       <c r="B87" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3046</v>
+        <v>3001</v>
+      </c>
+      <c r="C87" s="1">
+        <v>1086</v>
       </c>
       <c r="D87" s="1">
         <v>0</v>
@@ -14774,7 +15032,10 @@
       </c>
       <c r="B88" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3006</v>
+        <v>3071</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1087</v>
       </c>
       <c r="D88" s="1">
         <v>0</v>
@@ -14789,7 +15050,10 @@
       </c>
       <c r="B89" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3001</v>
+        <v>3046</v>
+      </c>
+      <c r="C89" s="1">
+        <v>1088</v>
       </c>
       <c r="D89" s="1">
         <v>0</v>
@@ -14804,7 +15068,10 @@
       </c>
       <c r="B90" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3076</v>
+        <v>3041</v>
+      </c>
+      <c r="C90" s="1">
+        <v>1089</v>
       </c>
       <c r="D90" s="1">
         <v>0</v>
@@ -14819,7 +15086,10 @@
       </c>
       <c r="B91" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3013</v>
+        <v>3053</v>
+      </c>
+      <c r="C91" s="1">
+        <v>1090</v>
       </c>
       <c r="D91" s="1">
         <v>0</v>
@@ -14834,7 +15104,10 @@
       </c>
       <c r="B92" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3067</v>
+        <v>3038</v>
+      </c>
+      <c r="C92" s="1">
+        <v>1091</v>
       </c>
       <c r="D92" s="1">
         <v>0</v>
@@ -14849,7 +15122,10 @@
       </c>
       <c r="B93" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3083</v>
+        <v>3048</v>
+      </c>
+      <c r="C93" s="1">
+        <v>1092</v>
       </c>
       <c r="D93" s="1">
         <v>0</v>
@@ -14864,7 +15140,10 @@
       </c>
       <c r="B94" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3002</v>
+        <v>3022</v>
+      </c>
+      <c r="C94" s="1">
+        <v>1093</v>
       </c>
       <c r="D94" s="1">
         <v>0</v>
@@ -14879,7 +15158,10 @@
       </c>
       <c r="B95" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3015</v>
+        <v>3019</v>
+      </c>
+      <c r="C95" s="1">
+        <v>1094</v>
       </c>
       <c r="D95" s="1">
         <v>0</v>
@@ -14894,7 +15176,10 @@
       </c>
       <c r="B96" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3011</v>
+        <v>3084</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1095</v>
       </c>
       <c r="D96" s="1">
         <v>0</v>
@@ -14909,7 +15194,10 @@
       </c>
       <c r="B97" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3061</v>
+        <v>3053</v>
+      </c>
+      <c r="C97" s="1">
+        <v>1096</v>
       </c>
       <c r="D97" s="1">
         <v>0</v>
@@ -14924,7 +15212,10 @@
       </c>
       <c r="B98" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3023</v>
+        <v>3037</v>
+      </c>
+      <c r="C98" s="1">
+        <v>1097</v>
       </c>
       <c r="D98" s="1">
         <v>0</v>
@@ -14939,7 +15230,10 @@
       </c>
       <c r="B99" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3083</v>
+        <v>3080</v>
+      </c>
+      <c r="C99" s="1">
+        <v>1098</v>
       </c>
       <c r="D99" s="1">
         <v>0</v>
@@ -14954,7 +15248,10 @@
       </c>
       <c r="B100" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3046</v>
+        <v>3027</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1099</v>
       </c>
       <c r="D100" s="1">
         <v>0</v>
@@ -14969,7 +15266,10 @@
       </c>
       <c r="B101" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3097</v>
+        <v>3036</v>
+      </c>
+      <c r="C101" s="1">
+        <v>1100</v>
       </c>
       <c r="D101" s="1">
         <v>0</v>
@@ -14984,7 +15284,10 @@
       </c>
       <c r="B102" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3045</v>
+        <v>3048</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1101</v>
       </c>
       <c r="D102" s="1">
         <v>0</v>
@@ -14999,7 +15302,10 @@
       </c>
       <c r="B103" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3085</v>
+        <v>3001</v>
+      </c>
+      <c r="C103" s="1">
+        <v>1102</v>
       </c>
       <c r="D103" s="1">
         <v>0</v>
@@ -15014,7 +15320,10 @@
       </c>
       <c r="B104" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3095</v>
+        <v>3004</v>
+      </c>
+      <c r="C104" s="1">
+        <v>1103</v>
       </c>
       <c r="D104" s="1">
         <v>0</v>
@@ -15029,7 +15338,10 @@
       </c>
       <c r="B105" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3095</v>
+        <v>3080</v>
+      </c>
+      <c r="C105" s="1">
+        <v>1104</v>
       </c>
       <c r="D105" s="1">
         <v>0</v>
@@ -15044,7 +15356,10 @@
       </c>
       <c r="B106" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3047</v>
+        <v>3013</v>
+      </c>
+      <c r="C106" s="1">
+        <v>1105</v>
       </c>
       <c r="D106" s="1">
         <v>0</v>
@@ -15059,7 +15374,10 @@
       </c>
       <c r="B107" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3050</v>
+        <v>3056</v>
+      </c>
+      <c r="C107" s="1">
+        <v>1106</v>
       </c>
       <c r="D107" s="1">
         <v>0</v>
@@ -15074,7 +15392,10 @@
       </c>
       <c r="B108" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3050</v>
+        <v>3097</v>
+      </c>
+      <c r="C108" s="1">
+        <v>1107</v>
       </c>
       <c r="D108" s="1">
         <v>0</v>
@@ -15089,7 +15410,10 @@
       </c>
       <c r="B109" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3020</v>
+        <v>3087</v>
+      </c>
+      <c r="C109" s="1">
+        <v>1108</v>
       </c>
       <c r="D109" s="1">
         <v>0</v>
@@ -15104,7 +15428,10 @@
       </c>
       <c r="B110" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3003</v>
+        <v>3049</v>
+      </c>
+      <c r="C110" s="1">
+        <v>1109</v>
       </c>
       <c r="D110" s="1">
         <v>0</v>

</xml_diff>